<commit_message>
print locations of all files in the report
</commit_message>
<xml_diff>
--- a/resources/templates/report-template.xlsx
+++ b/resources/templates/report-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NicHaydel\workspace\cdisc-rules-engine\resources\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aleksei_Furmenkov/PycharmProjects/cdisc-rules-engine/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9509EF25-588A-4E23-842E-508D6784CC6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA74DB7D-5DCF-0240-BC65-95FD35A8802B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4DEAAD2A-344E-470C-8C9E-CF593FD647F4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{4DEAAD2A-344E-470C-8C9E-CF593FD647F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Conformance Details" sheetId="4" r:id="rId1"/>
@@ -198,15 +198,26 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="25">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -226,6 +237,51 @@
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -257,6 +313,12 @@
           <bgColor rgb="FF40B4E5"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -313,73 +375,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFCCE6E3"/>
         </patternFill>
       </fill>
@@ -394,8 +389,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="CDISC" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="CDISC" pivot="0" count="2" xr9:uid="{69FBD606-89C9-4CBA-9BEE-430778E41327}">
-      <tableStyleElement type="headerRow" dxfId="25"/>
-      <tableStyleElement type="secondRowStripe" dxfId="24"/>
+      <tableStyleElement type="headerRow" dxfId="24"/>
+      <tableStyleElement type="secondRowStripe" dxfId="23"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -430,8 +425,8 @@
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A4677B52-4485-485A-BFC5-88C68D89C965}" name="Dataset"/>
-    <tableColumn id="2" xr3:uid="{FBDFFB0A-6A65-40F7-B7C1-B92B010FBEC9}" name="RuleID" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{3B15064B-7E09-480E-B63C-E93ACA503094}" name="Message" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{FBDFFB0A-6A65-40F7-B7C1-B92B010FBEC9}" name="RuleID" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{3B15064B-7E09-480E-B63C-E93ACA503094}" name="Message" dataDxfId="14"/>
     <tableColumn id="4" xr3:uid="{F96B2454-B4BC-41CF-97D6-354BF7DA658C}" name="Severity"/>
     <tableColumn id="5" xr3:uid="{A33A2D5F-ED56-4ACA-BDB5-A3B54FDFFE4F}" name="Issues"/>
     <tableColumn id="6" xr3:uid="{A33654D2-16F9-4A4C-9ACE-EA3650900336}" name="Explanation"/>
@@ -449,15 +444,15 @@
     <sortCondition ref="E2:E150"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E14C5FBE-76D0-4D41-B4DD-8BBF28D09E06}" name="RuleID" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{36A516EC-8CA6-446B-931B-6DD60430F605}" name="Message" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{E14C5FBE-76D0-4D41-B4DD-8BBF28D09E06}" name="RuleID" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{36A516EC-8CA6-446B-931B-6DD60430F605}" name="Message" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{685E7B09-FB5C-4523-8ACB-8B50A8BDD7CB}" name="Severity"/>
     <tableColumn id="4" xr3:uid="{8C809B58-A492-4607-8E72-ED606C841C08}" name="Dataset"/>
     <tableColumn id="5" xr3:uid="{AE7926B7-2872-4A2D-B8DD-CD01A3BC9436}" name="USUBJID"/>
-    <tableColumn id="6" xr3:uid="{0451A533-75C9-49B3-8DDF-A664E805E30A}" name="Record" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{0451A533-75C9-49B3-8DDF-A664E805E30A}" name="Record" dataDxfId="7"/>
     <tableColumn id="7" xr3:uid="{2EC1BE1B-03B8-4035-A6CF-A6F5E7F6ED73}" name="Sequence"/>
-    <tableColumn id="8" xr3:uid="{914E2604-487C-459B-A24D-F233F0858683}" name="Variable(s)" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{19271926-2DDD-4702-94B1-2D701B30975B}" name="Value(s)" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{914E2604-487C-459B-A24D-F233F0858683}" name="Variable(s)" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{19271926-2DDD-4702-94B1-2D701B30975B}" name="Value(s)" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -467,10 +462,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}" name="Table2" displayName="Table2" ref="A1:D200" totalsRowShown="0">
   <autoFilter ref="A1:D200" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3C4707C1-408B-4B6A-B278-5F3FA8733BBE}" name="RuleID" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{3C4707C1-408B-4B6A-B278-5F3FA8733BBE}" name="RuleID" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{B88367B4-F155-408A-9DD0-DD0E99F112AE}" name="Version"/>
-    <tableColumn id="2" xr3:uid="{676B4D84-CB39-48B1-86C4-12E66A4FBF76}" name="Message" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{2C710F94-A29A-4635-BD01-2691D10AF83B}" name="Status" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{676B4D84-CB39-48B1-86C4-12E66A4FBF76}" name="Message" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{2C710F94-A29A-4635-BD01-2691D10AF83B}" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -776,27 +771,27 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="82.42578125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="82.5" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="8"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -804,21 +799,21 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="8"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="7"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -826,7 +821,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -834,7 +829,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -842,7 +837,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
@@ -850,7 +845,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
@@ -858,7 +853,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -866,7 +861,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
@@ -874,7 +869,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
@@ -882,7 +877,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
@@ -896,17 +891,17 @@
     <mergeCell ref="A7:B7"/>
   </mergeCells>
   <conditionalFormatting sqref="B17:B1048576 A7 B1:B2 B4:B6">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B16">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -923,17 +918,17 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="72.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="72.5" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="76.28515625" customWidth="1"/>
+    <col min="6" max="6" width="76.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -953,255 +948,254 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
       <formula>"notice"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
       <formula>"warning"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
       <formula>"Reject"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
       <formula>"error"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1225,20 +1219,20 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="64.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="64.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1267,769 +1261,769 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="F3" s="2"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="F4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="F5" s="2"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="F6" s="2"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="F7" s="2"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="F8" s="2"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="F9" s="2"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="F10" s="2"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="F39" s="2"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="F45" s="2"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="F47" s="2"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="F49" s="2"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="F51" s="2"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="F53" s="2"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="F54" s="2"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="F55" s="2"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="F56" s="2"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="F57" s="2"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="F58" s="2"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="F59" s="2"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="F61" s="2"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="F62" s="2"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="F63" s="2"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="F64" s="2"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="F66" s="2"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="F67" s="2"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="F68" s="2"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="F70" s="2"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="F72" s="2"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="F73" s="2"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="F74" s="2"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="F75" s="2"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="F76" s="2"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="F77" s="2"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="F78" s="2"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="F79" s="2"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="F80" s="2"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="F81" s="2"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="F82" s="2"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="F83" s="2"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="F84" s="2"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="F85" s="2"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="F86" s="2"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="F87" s="2"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="F88" s="2"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="F89" s="2"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="F90" s="2"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="F91" s="2"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="F92" s="2"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="F93" s="2"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="F94" s="2"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="F95" s="2"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="F96" s="2"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="F97" s="2"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="F98" s="2"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="F99" s="2"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="F100" s="2"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="1"/>
       <c r="B101" s="2"/>
       <c r="F101" s="2"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="1"/>
       <c r="B102" s="2"/>
       <c r="F102" s="2"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="1"/>
       <c r="B103" s="2"/>
       <c r="F103" s="2"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="1"/>
       <c r="B104" s="2"/>
       <c r="F104" s="2"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
       <c r="B105" s="2"/>
       <c r="F105" s="2"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="1"/>
       <c r="B106" s="2"/>
       <c r="F106" s="2"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="1"/>
       <c r="B107" s="2"/>
       <c r="F107" s="2"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="1"/>
       <c r="B108" s="2"/>
       <c r="F108" s="2"/>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="1"/>
       <c r="B109" s="2"/>
       <c r="F109" s="2"/>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="1"/>
       <c r="B110" s="2"/>
       <c r="F110" s="2"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="1"/>
       <c r="B111" s="2"/>
       <c r="F111" s="2"/>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="1"/>
       <c r="B112" s="2"/>
       <c r="F112" s="2"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="1"/>
       <c r="B113" s="2"/>
       <c r="F113" s="2"/>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="1"/>
       <c r="B114" s="2"/>
       <c r="F114" s="2"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="1"/>
       <c r="B115" s="2"/>
       <c r="F115" s="2"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="1"/>
       <c r="B116" s="2"/>
       <c r="F116" s="2"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="1"/>
       <c r="B117" s="2"/>
       <c r="F117" s="2"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="1"/>
       <c r="B118" s="2"/>
       <c r="F118" s="2"/>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="1"/>
       <c r="B119" s="2"/>
       <c r="F119" s="2"/>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="1"/>
       <c r="B120" s="2"/>
       <c r="F120" s="2"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="1"/>
       <c r="B121" s="2"/>
       <c r="F121" s="2"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="1"/>
       <c r="B122" s="2"/>
       <c r="F122" s="2"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="1"/>
       <c r="B123" s="2"/>
       <c r="F123" s="2"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="1"/>
       <c r="B124" s="2"/>
       <c r="F124" s="2"/>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="1"/>
       <c r="B125" s="2"/>
       <c r="F125" s="2"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="1"/>
       <c r="B126" s="2"/>
       <c r="F126" s="2"/>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="1"/>
       <c r="B127" s="2"/>
       <c r="F127" s="2"/>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="1"/>
       <c r="B128" s="2"/>
       <c r="F128" s="2"/>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" s="1"/>
       <c r="B129" s="2"/>
       <c r="F129" s="2"/>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" s="1"/>
       <c r="B130" s="2"/>
       <c r="F130" s="2"/>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="1"/>
       <c r="B131" s="2"/>
       <c r="F131" s="2"/>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="1"/>
       <c r="B132" s="2"/>
       <c r="F132" s="2"/>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="1"/>
       <c r="B133" s="2"/>
       <c r="F133" s="2"/>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" s="1"/>
       <c r="B134" s="2"/>
       <c r="F134" s="2"/>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" s="1"/>
       <c r="B135" s="2"/>
       <c r="F135" s="2"/>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" s="1"/>
       <c r="B136" s="2"/>
       <c r="F136" s="2"/>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" s="1"/>
       <c r="B137" s="2"/>
       <c r="F137" s="2"/>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="1"/>
       <c r="B138" s="2"/>
       <c r="F138" s="2"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="1"/>
       <c r="B139" s="2"/>
       <c r="F139" s="2"/>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" s="1"/>
       <c r="B140" s="2"/>
       <c r="F140" s="2"/>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" s="1"/>
       <c r="B141" s="2"/>
       <c r="F141" s="2"/>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" s="1"/>
       <c r="B142" s="2"/>
       <c r="F142" s="2"/>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" s="1"/>
       <c r="B143" s="2"/>
       <c r="F143" s="2"/>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" s="1"/>
       <c r="B144" s="2"/>
       <c r="F144" s="2"/>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="1"/>
       <c r="B145" s="2"/>
       <c r="F145" s="2"/>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" s="1"/>
       <c r="B146" s="2"/>
       <c r="F146" s="2"/>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" s="1"/>
       <c r="B147" s="2"/>
       <c r="F147" s="2"/>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="1"/>
       <c r="B148" s="2"/>
       <c r="F148" s="2"/>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" s="1"/>
       <c r="B149" s="2"/>
       <c r="F149" s="2"/>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" s="1"/>
       <c r="B150" s="2"/>
       <c r="F150" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"Notice"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"Warning"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>"Reject"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2053,15 +2047,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="43.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="43.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="100" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2075,609 +2069,609 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" s="1"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" s="1"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" s="1"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" s="1"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" s="1"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" s="1"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" s="1"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" s="1"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" s="1"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" s="1"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" s="1"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" s="1"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" s="1"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" s="1"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" s="1"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" s="1"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" s="1"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" s="1"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" s="1"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" s="1"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" s="1"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" s="1"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" s="1"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" s="1"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" s="1"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" s="1"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" s="1"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" s="1"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" s="1"/>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" s="1"/>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" s="1"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" s="1"/>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" s="1"/>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" s="1"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" s="1"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" s="1"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" s="1"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" s="1"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" s="1"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" s="1"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" s="1"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" s="1"/>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" s="1"/>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" s="1"/>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" s="1"/>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" s="1"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" s="1"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" s="1"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" s="1"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" s="1"/>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" s="1"/>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" s="1"/>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" s="1"/>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" s="1"/>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" s="1"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" s="1"/>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" s="1"/>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" s="1"/>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" s="1"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" s="1"/>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" s="1"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" s="1"/>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" s="1"/>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" s="1"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" s="1"/>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" s="1"/>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" s="1"/>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" s="1"/>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" s="1"/>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" s="1"/>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" s="1"/>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" s="1"/>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" s="1"/>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" s="1"/>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" s="1"/>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" s="1"/>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" s="1"/>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" s="1"/>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" s="1"/>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" s="1"/>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" s="1"/>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" s="1"/>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" s="1"/>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" s="1"/>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" s="1"/>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" s="1"/>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" s="1"/>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" s="1"/>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" s="1"/>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" s="1"/>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" s="1"/>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" s="1"/>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" s="1"/>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" s="1"/>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" s="1"/>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" s="1"/>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" s="1"/>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" s="1"/>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" s="1"/>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" s="1"/>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" s="1"/>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" s="1"/>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" s="1"/>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" s="1"/>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" s="1"/>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"SUCCESS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add all keyword, and update rule transformation logic
</commit_message>
<xml_diff>
--- a/resources/templates/report-template.xlsx
+++ b/resources/templates/report-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aleksei_Furmenkov/PycharmProjects/cdisc-rules-engine/resources/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NicHaydel\workspace\cdisc-rules-engine\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA74DB7D-5DCF-0240-BC65-95FD35A8802B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854E8589-3490-4F3A-8B61-AD76AA939DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{4DEAAD2A-344E-470C-8C9E-CF593FD647F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{4DEAAD2A-344E-470C-8C9E-CF593FD647F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Conformance Details" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Dataset</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Data Location</t>
+  </si>
+  <si>
+    <t>Executability</t>
   </si>
 </sst>
 </file>
@@ -198,26 +201,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="25">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -237,51 +231,6 @@
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -313,12 +262,6 @@
           <bgColor rgb="FF40B4E5"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -373,6 +316,66 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFCCE6E3"/>
@@ -425,8 +428,8 @@
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A4677B52-4485-485A-BFC5-88C68D89C965}" name="Dataset"/>
-    <tableColumn id="2" xr3:uid="{FBDFFB0A-6A65-40F7-B7C1-B92B010FBEC9}" name="RuleID" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{3B15064B-7E09-480E-B63C-E93ACA503094}" name="Message" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{FBDFFB0A-6A65-40F7-B7C1-B92B010FBEC9}" name="RuleID" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{3B15064B-7E09-480E-B63C-E93ACA503094}" name="Message" dataDxfId="21"/>
     <tableColumn id="4" xr3:uid="{F96B2454-B4BC-41CF-97D6-354BF7DA658C}" name="Severity"/>
     <tableColumn id="5" xr3:uid="{A33A2D5F-ED56-4ACA-BDB5-A3B54FDFFE4F}" name="Issues"/>
     <tableColumn id="6" xr3:uid="{A33654D2-16F9-4A4C-9ACE-EA3650900336}" name="Explanation"/>
@@ -444,15 +447,15 @@
     <sortCondition ref="E2:E150"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E14C5FBE-76D0-4D41-B4DD-8BBF28D09E06}" name="RuleID" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{36A516EC-8CA6-446B-931B-6DD60430F605}" name="Message" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{685E7B09-FB5C-4523-8ACB-8B50A8BDD7CB}" name="Severity"/>
+    <tableColumn id="1" xr3:uid="{E14C5FBE-76D0-4D41-B4DD-8BBF28D09E06}" name="RuleID" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{36A516EC-8CA6-446B-931B-6DD60430F605}" name="Message" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{685E7B09-FB5C-4523-8ACB-8B50A8BDD7CB}" name="Executability"/>
     <tableColumn id="4" xr3:uid="{8C809B58-A492-4607-8E72-ED606C841C08}" name="Dataset"/>
     <tableColumn id="5" xr3:uid="{AE7926B7-2872-4A2D-B8DD-CD01A3BC9436}" name="USUBJID"/>
-    <tableColumn id="6" xr3:uid="{0451A533-75C9-49B3-8DDF-A664E805E30A}" name="Record" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{0451A533-75C9-49B3-8DDF-A664E805E30A}" name="Record" dataDxfId="18"/>
     <tableColumn id="7" xr3:uid="{2EC1BE1B-03B8-4035-A6CF-A6F5E7F6ED73}" name="Sequence"/>
-    <tableColumn id="8" xr3:uid="{914E2604-487C-459B-A24D-F233F0858683}" name="Variable(s)" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{19271926-2DDD-4702-94B1-2D701B30975B}" name="Value(s)" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{914E2604-487C-459B-A24D-F233F0858683}" name="Variable(s)" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{19271926-2DDD-4702-94B1-2D701B30975B}" name="Value(s)" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -462,10 +465,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}" name="Table2" displayName="Table2" ref="A1:D200" totalsRowShown="0">
   <autoFilter ref="A1:D200" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3C4707C1-408B-4B6A-B278-5F3FA8733BBE}" name="RuleID" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{3C4707C1-408B-4B6A-B278-5F3FA8733BBE}" name="RuleID" dataDxfId="15"/>
     <tableColumn id="4" xr3:uid="{B88367B4-F155-408A-9DD0-DD0E99F112AE}" name="Version"/>
-    <tableColumn id="2" xr3:uid="{676B4D84-CB39-48B1-86C4-12E66A4FBF76}" name="Message" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{2C710F94-A29A-4635-BD01-2691D10AF83B}" name="Status" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{676B4D84-CB39-48B1-86C4-12E66A4FBF76}" name="Message" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{2C710F94-A29A-4635-BD01-2691D10AF83B}" name="Status" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -770,28 +773,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D798A9F-8AC0-4EAA-BD02-664438CF629A}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5" customWidth="1"/>
-    <col min="2" max="2" width="82.5" style="5" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="82.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="7"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="B1" s="8"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -799,21 +802,21 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="7"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" s="8"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -821,7 +824,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -829,7 +832,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -837,7 +840,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
@@ -845,7 +848,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
@@ -853,7 +856,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -861,7 +864,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
@@ -869,7 +872,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
@@ -877,7 +880,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
@@ -891,17 +894,17 @@
     <mergeCell ref="A7:B7"/>
   </mergeCells>
   <conditionalFormatting sqref="B17:B1048576 A7 B1:B2 B4:B6">
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B16">
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -918,17 +921,17 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="72.5" customWidth="1"/>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="72.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="76.33203125" customWidth="1"/>
+    <col min="6" max="6" width="76.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -948,254 +951,254 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"notice"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"warning"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"Reject"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"error"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1215,24 +1218,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F51C09C-55A4-4B8A-87C6-1EAF95BD08E9}">
   <dimension ref="A1:I150"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="64.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="64.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1240,7 +1243,7 @@
         <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1261,769 +1264,769 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="F3" s="2"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="F4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="F5" s="2"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="F6" s="2"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="F7" s="2"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="F8" s="2"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="F9" s="2"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="F10" s="2"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="F39" s="2"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="F45" s="2"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="F47" s="2"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="F49" s="2"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="F51" s="2"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="F53" s="2"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="F54" s="2"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="F55" s="2"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="F56" s="2"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="F57" s="2"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="F58" s="2"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="F59" s="2"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="F61" s="2"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="F62" s="2"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="F63" s="2"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="F64" s="2"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="F66" s="2"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="F67" s="2"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="F68" s="2"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="F70" s="2"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="F72" s="2"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="F73" s="2"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="F74" s="2"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="F75" s="2"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="F76" s="2"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="F77" s="2"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="F78" s="2"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="F79" s="2"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="F80" s="2"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="F81" s="2"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="F82" s="2"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="F83" s="2"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="F84" s="2"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="F85" s="2"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="F86" s="2"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="F87" s="2"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="F88" s="2"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="F89" s="2"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="F90" s="2"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="F91" s="2"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="F92" s="2"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="F93" s="2"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="F94" s="2"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="F95" s="2"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="F96" s="2"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="F97" s="2"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="F98" s="2"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="F99" s="2"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="F100" s="2"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="2"/>
       <c r="F101" s="2"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="2"/>
       <c r="F102" s="2"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="2"/>
       <c r="F103" s="2"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="2"/>
       <c r="F104" s="2"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="2"/>
       <c r="F105" s="2"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="2"/>
       <c r="F106" s="2"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="2"/>
       <c r="F107" s="2"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="2"/>
       <c r="F108" s="2"/>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="2"/>
       <c r="F109" s="2"/>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="2"/>
       <c r="F110" s="2"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="2"/>
       <c r="F111" s="2"/>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="2"/>
       <c r="F112" s="2"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="2"/>
       <c r="F113" s="2"/>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="2"/>
       <c r="F114" s="2"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="2"/>
       <c r="F115" s="2"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="2"/>
       <c r="F116" s="2"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="2"/>
       <c r="F117" s="2"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="2"/>
       <c r="F118" s="2"/>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="2"/>
       <c r="F119" s="2"/>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="2"/>
       <c r="F120" s="2"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="2"/>
       <c r="F121" s="2"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="2"/>
       <c r="F122" s="2"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="2"/>
       <c r="F123" s="2"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="2"/>
       <c r="F124" s="2"/>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="2"/>
       <c r="F125" s="2"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="2"/>
       <c r="F126" s="2"/>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="2"/>
       <c r="F127" s="2"/>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="2"/>
       <c r="F128" s="2"/>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="2"/>
       <c r="F129" s="2"/>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="2"/>
       <c r="F130" s="2"/>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="2"/>
       <c r="F131" s="2"/>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="2"/>
       <c r="F132" s="2"/>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="2"/>
       <c r="F133" s="2"/>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="2"/>
       <c r="F134" s="2"/>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="2"/>
       <c r="F135" s="2"/>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="2"/>
       <c r="F136" s="2"/>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="2"/>
       <c r="F137" s="2"/>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="2"/>
       <c r="F138" s="2"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="2"/>
       <c r="F139" s="2"/>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="2"/>
       <c r="F140" s="2"/>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="2"/>
       <c r="F141" s="2"/>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="2"/>
       <c r="F142" s="2"/>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="2"/>
       <c r="F143" s="2"/>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="2"/>
       <c r="F144" s="2"/>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="2"/>
       <c r="F145" s="2"/>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="2"/>
       <c r="F146" s="2"/>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="2"/>
       <c r="F147" s="2"/>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="2"/>
       <c r="F148" s="2"/>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="2"/>
       <c r="F149" s="2"/>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="2"/>
       <c r="F150" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Notice"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Warning"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Reject"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2047,15 +2050,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="43.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="43.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="100" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2069,609 +2072,609 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"SUCCESS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Rule schema updates (#246)
* Add all keyword, and update rule transformation logic

* update cache with rules using new schema

* Latest cache update

* Update version and rules cache
</commit_message>
<xml_diff>
--- a/resources/templates/report-template.xlsx
+++ b/resources/templates/report-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aleksei_Furmenkov/PycharmProjects/cdisc-rules-engine/resources/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NicHaydel\workspace\cdisc-rules-engine\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA74DB7D-5DCF-0240-BC65-95FD35A8802B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854E8589-3490-4F3A-8B61-AD76AA939DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{4DEAAD2A-344E-470C-8C9E-CF593FD647F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{4DEAAD2A-344E-470C-8C9E-CF593FD647F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Conformance Details" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Dataset</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Data Location</t>
+  </si>
+  <si>
+    <t>Executability</t>
   </si>
 </sst>
 </file>
@@ -198,26 +201,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="25">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -237,51 +231,6 @@
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -313,12 +262,6 @@
           <bgColor rgb="FF40B4E5"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -373,6 +316,66 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFCCE6E3"/>
@@ -425,8 +428,8 @@
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A4677B52-4485-485A-BFC5-88C68D89C965}" name="Dataset"/>
-    <tableColumn id="2" xr3:uid="{FBDFFB0A-6A65-40F7-B7C1-B92B010FBEC9}" name="RuleID" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{3B15064B-7E09-480E-B63C-E93ACA503094}" name="Message" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{FBDFFB0A-6A65-40F7-B7C1-B92B010FBEC9}" name="RuleID" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{3B15064B-7E09-480E-B63C-E93ACA503094}" name="Message" dataDxfId="21"/>
     <tableColumn id="4" xr3:uid="{F96B2454-B4BC-41CF-97D6-354BF7DA658C}" name="Severity"/>
     <tableColumn id="5" xr3:uid="{A33A2D5F-ED56-4ACA-BDB5-A3B54FDFFE4F}" name="Issues"/>
     <tableColumn id="6" xr3:uid="{A33654D2-16F9-4A4C-9ACE-EA3650900336}" name="Explanation"/>
@@ -444,15 +447,15 @@
     <sortCondition ref="E2:E150"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E14C5FBE-76D0-4D41-B4DD-8BBF28D09E06}" name="RuleID" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{36A516EC-8CA6-446B-931B-6DD60430F605}" name="Message" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{685E7B09-FB5C-4523-8ACB-8B50A8BDD7CB}" name="Severity"/>
+    <tableColumn id="1" xr3:uid="{E14C5FBE-76D0-4D41-B4DD-8BBF28D09E06}" name="RuleID" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{36A516EC-8CA6-446B-931B-6DD60430F605}" name="Message" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{685E7B09-FB5C-4523-8ACB-8B50A8BDD7CB}" name="Executability"/>
     <tableColumn id="4" xr3:uid="{8C809B58-A492-4607-8E72-ED606C841C08}" name="Dataset"/>
     <tableColumn id="5" xr3:uid="{AE7926B7-2872-4A2D-B8DD-CD01A3BC9436}" name="USUBJID"/>
-    <tableColumn id="6" xr3:uid="{0451A533-75C9-49B3-8DDF-A664E805E30A}" name="Record" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{0451A533-75C9-49B3-8DDF-A664E805E30A}" name="Record" dataDxfId="18"/>
     <tableColumn id="7" xr3:uid="{2EC1BE1B-03B8-4035-A6CF-A6F5E7F6ED73}" name="Sequence"/>
-    <tableColumn id="8" xr3:uid="{914E2604-487C-459B-A24D-F233F0858683}" name="Variable(s)" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{19271926-2DDD-4702-94B1-2D701B30975B}" name="Value(s)" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{914E2604-487C-459B-A24D-F233F0858683}" name="Variable(s)" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{19271926-2DDD-4702-94B1-2D701B30975B}" name="Value(s)" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -462,10 +465,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}" name="Table2" displayName="Table2" ref="A1:D200" totalsRowShown="0">
   <autoFilter ref="A1:D200" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3C4707C1-408B-4B6A-B278-5F3FA8733BBE}" name="RuleID" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{3C4707C1-408B-4B6A-B278-5F3FA8733BBE}" name="RuleID" dataDxfId="15"/>
     <tableColumn id="4" xr3:uid="{B88367B4-F155-408A-9DD0-DD0E99F112AE}" name="Version"/>
-    <tableColumn id="2" xr3:uid="{676B4D84-CB39-48B1-86C4-12E66A4FBF76}" name="Message" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{2C710F94-A29A-4635-BD01-2691D10AF83B}" name="Status" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{676B4D84-CB39-48B1-86C4-12E66A4FBF76}" name="Message" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{2C710F94-A29A-4635-BD01-2691D10AF83B}" name="Status" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -770,28 +773,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D798A9F-8AC0-4EAA-BD02-664438CF629A}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5" customWidth="1"/>
-    <col min="2" max="2" width="82.5" style="5" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="82.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="7"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="B1" s="8"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -799,21 +802,21 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="7"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" s="8"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -821,7 +824,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -829,7 +832,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -837,7 +840,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
@@ -845,7 +848,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
@@ -853,7 +856,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -861,7 +864,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
@@ -869,7 +872,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
@@ -877,7 +880,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
@@ -891,17 +894,17 @@
     <mergeCell ref="A7:B7"/>
   </mergeCells>
   <conditionalFormatting sqref="B17:B1048576 A7 B1:B2 B4:B6">
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B16">
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -918,17 +921,17 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="72.5" customWidth="1"/>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="72.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="76.33203125" customWidth="1"/>
+    <col min="6" max="6" width="76.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -948,254 +951,254 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"notice"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"warning"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"Reject"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"error"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1215,24 +1218,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F51C09C-55A4-4B8A-87C6-1EAF95BD08E9}">
   <dimension ref="A1:I150"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="64.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="64.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1240,7 +1243,7 @@
         <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1261,769 +1264,769 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="F3" s="2"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="F4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="F5" s="2"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="F6" s="2"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="F7" s="2"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="F8" s="2"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="F9" s="2"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="F10" s="2"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="F39" s="2"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="F45" s="2"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="F47" s="2"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="F49" s="2"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="F51" s="2"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="F53" s="2"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="F54" s="2"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="F55" s="2"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="F56" s="2"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="F57" s="2"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="F58" s="2"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="F59" s="2"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="F61" s="2"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="F62" s="2"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
       <c r="F63" s="2"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="F64" s="2"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
       <c r="F66" s="2"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
       <c r="F67" s="2"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
       <c r="F68" s="2"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="F70" s="2"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="F72" s="2"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
       <c r="F73" s="2"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
       <c r="F74" s="2"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="F75" s="2"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="F76" s="2"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
       <c r="F77" s="2"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
       <c r="F78" s="2"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
       <c r="F79" s="2"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
       <c r="F80" s="2"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
       <c r="F81" s="2"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
       <c r="F82" s="2"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
       <c r="F83" s="2"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="F84" s="2"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="F85" s="2"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="F86" s="2"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
       <c r="F87" s="2"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
       <c r="F88" s="2"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
       <c r="F89" s="2"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
       <c r="F90" s="2"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
       <c r="F91" s="2"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
       <c r="F92" s="2"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
       <c r="F93" s="2"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
       <c r="F94" s="2"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="F95" s="2"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="F96" s="2"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="F97" s="2"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
       <c r="F98" s="2"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
       <c r="F99" s="2"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
       <c r="F100" s="2"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="2"/>
       <c r="F101" s="2"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="2"/>
       <c r="F102" s="2"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="2"/>
       <c r="F103" s="2"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="2"/>
       <c r="F104" s="2"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="2"/>
       <c r="F105" s="2"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="2"/>
       <c r="F106" s="2"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="2"/>
       <c r="F107" s="2"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="2"/>
       <c r="F108" s="2"/>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="2"/>
       <c r="F109" s="2"/>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="2"/>
       <c r="F110" s="2"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="2"/>
       <c r="F111" s="2"/>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="2"/>
       <c r="F112" s="2"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="2"/>
       <c r="F113" s="2"/>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="2"/>
       <c r="F114" s="2"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="2"/>
       <c r="F115" s="2"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="2"/>
       <c r="F116" s="2"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="2"/>
       <c r="F117" s="2"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="2"/>
       <c r="F118" s="2"/>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="2"/>
       <c r="F119" s="2"/>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="2"/>
       <c r="F120" s="2"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="2"/>
       <c r="F121" s="2"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="2"/>
       <c r="F122" s="2"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="2"/>
       <c r="F123" s="2"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="2"/>
       <c r="F124" s="2"/>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="2"/>
       <c r="F125" s="2"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="2"/>
       <c r="F126" s="2"/>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="2"/>
       <c r="F127" s="2"/>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="2"/>
       <c r="F128" s="2"/>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="2"/>
       <c r="F129" s="2"/>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="2"/>
       <c r="F130" s="2"/>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="2"/>
       <c r="F131" s="2"/>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="2"/>
       <c r="F132" s="2"/>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="2"/>
       <c r="F133" s="2"/>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="2"/>
       <c r="F134" s="2"/>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="2"/>
       <c r="F135" s="2"/>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="2"/>
       <c r="F136" s="2"/>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="2"/>
       <c r="F137" s="2"/>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="2"/>
       <c r="F138" s="2"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="2"/>
       <c r="F139" s="2"/>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="2"/>
       <c r="F140" s="2"/>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="2"/>
       <c r="F141" s="2"/>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="2"/>
       <c r="F142" s="2"/>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="2"/>
       <c r="F143" s="2"/>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="2"/>
       <c r="F144" s="2"/>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="2"/>
       <c r="F145" s="2"/>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="2"/>
       <c r="F146" s="2"/>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="2"/>
       <c r="F147" s="2"/>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="2"/>
       <c r="F148" s="2"/>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="2"/>
       <c r="F149" s="2"/>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="2"/>
       <c r="F150" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Notice"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Warning"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Reject"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2047,15 +2050,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="43.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="43.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="100" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2069,609 +2072,609 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"SUCCESS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Uses new report template and fixes missing details
</commit_message>
<xml_diff>
--- a/resources/templates/report-template.xlsx
+++ b/resources/templates/report-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NicHaydel\workspace\cdisc-rules-engine\resources\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bdbelux1-my.sharepoint.com/personal/ndedonder_cro_brussels/Documents/CDISC/CORE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854E8589-3490-4F3A-8B61-AD76AA939DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{BAD70332-1D19-41D1-B6FD-7F9B6B2A0CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F789239-7438-4617-9285-8C33FE2CA11B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{4DEAAD2A-344E-470C-8C9E-CF593FD647F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{4DEAAD2A-344E-470C-8C9E-CF593FD647F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Conformance Details" sheetId="4" r:id="rId1"/>
@@ -37,17 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>Dataset</t>
   </si>
   <si>
-    <t>RuleID</t>
-  </si>
-  <si>
-    <t>Severity</t>
-  </si>
-  <si>
     <t>Explanation</t>
   </si>
   <si>
@@ -111,9 +105,6 @@
     <t>Not configured</t>
   </si>
   <si>
-    <t>Bundle Details</t>
-  </si>
-  <si>
     <t>Define-XML Version</t>
   </si>
   <si>
@@ -132,10 +123,25 @@
     <t>Total Runtime</t>
   </si>
   <si>
+    <t>Executability</t>
+  </si>
+  <si>
+    <t>Standards Details</t>
+  </si>
+  <si>
+    <t>CDISC RuleID</t>
+  </si>
+  <si>
+    <t>FDA RuleID</t>
+  </si>
+  <si>
+    <t>PMDA RuleID</t>
+  </si>
+  <si>
+    <t>CORE-ID</t>
+  </si>
+  <si>
     <t>Data Location</t>
-  </si>
-  <si>
-    <t>Executability</t>
   </si>
 </sst>
 </file>
@@ -187,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -201,9 +207,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -211,7 +214,16 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="21">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -231,98 +243,6 @@
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEDAA00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF40B4E5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEDAA00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF40B4E5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -370,10 +290,62 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDAA00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF40B4E5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -392,8 +364,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="CDISC" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="CDISC" pivot="0" count="2" xr9:uid="{69FBD606-89C9-4CBA-9BEE-430778E41327}">
-      <tableStyleElement type="headerRow" dxfId="24"/>
-      <tableStyleElement type="secondRowStripe" dxfId="23"/>
+      <tableStyleElement type="headerRow" dxfId="20"/>
+      <tableStyleElement type="secondRowStripe" dxfId="19"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -420,17 +392,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{91AB200C-AD87-44CC-B595-CF7F97FFAE49}" name="Table3" displayName="Table3" ref="A1:F60" totalsRowShown="0">
-  <autoFilter ref="A1:F60" xr:uid="{91AB200C-AD87-44CC-B595-CF7F97FFAE49}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{91AB200C-AD87-44CC-B595-CF7F97FFAE49}" name="Table3" displayName="Table3" ref="A1:E60" totalsRowShown="0">
+  <autoFilter ref="A1:E60" xr:uid="{91AB200C-AD87-44CC-B595-CF7F97FFAE49}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A2"/>
     <sortCondition ref="B2"/>
   </sortState>
-  <tableColumns count="6">
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{A4677B52-4485-485A-BFC5-88C68D89C965}" name="Dataset"/>
-    <tableColumn id="2" xr3:uid="{FBDFFB0A-6A65-40F7-B7C1-B92B010FBEC9}" name="RuleID" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{3B15064B-7E09-480E-B63C-E93ACA503094}" name="Message" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{F96B2454-B4BC-41CF-97D6-354BF7DA658C}" name="Severity"/>
+    <tableColumn id="2" xr3:uid="{FBDFFB0A-6A65-40F7-B7C1-B92B010FBEC9}" name="CORE-ID" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{3B15064B-7E09-480E-B63C-E93ACA503094}" name="Message" dataDxfId="14"/>
     <tableColumn id="5" xr3:uid="{A33A2D5F-ED56-4ACA-BDB5-A3B54FDFFE4F}" name="Issues"/>
     <tableColumn id="6" xr3:uid="{A33654D2-16F9-4A4C-9ACE-EA3650900336}" name="Explanation"/>
   </tableColumns>
@@ -447,28 +418,31 @@
     <sortCondition ref="E2:E150"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E14C5FBE-76D0-4D41-B4DD-8BBF28D09E06}" name="RuleID" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{36A516EC-8CA6-446B-931B-6DD60430F605}" name="Message" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{E14C5FBE-76D0-4D41-B4DD-8BBF28D09E06}" name="CORE-ID" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{36A516EC-8CA6-446B-931B-6DD60430F605}" name="Message" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{685E7B09-FB5C-4523-8ACB-8B50A8BDD7CB}" name="Executability"/>
     <tableColumn id="4" xr3:uid="{8C809B58-A492-4607-8E72-ED606C841C08}" name="Dataset"/>
     <tableColumn id="5" xr3:uid="{AE7926B7-2872-4A2D-B8DD-CD01A3BC9436}" name="USUBJID"/>
-    <tableColumn id="6" xr3:uid="{0451A533-75C9-49B3-8DDF-A664E805E30A}" name="Record" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{0451A533-75C9-49B3-8DDF-A664E805E30A}" name="Record" dataDxfId="7"/>
     <tableColumn id="7" xr3:uid="{2EC1BE1B-03B8-4035-A6CF-A6F5E7F6ED73}" name="Sequence"/>
-    <tableColumn id="8" xr3:uid="{914E2604-487C-459B-A24D-F233F0858683}" name="Variable(s)" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{19271926-2DDD-4702-94B1-2D701B30975B}" name="Value(s)" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{914E2604-487C-459B-A24D-F233F0858683}" name="Variable(s)" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{19271926-2DDD-4702-94B1-2D701B30975B}" name="Value(s)" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}" name="Table2" displayName="Table2" ref="A1:D200" totalsRowShown="0">
-  <autoFilter ref="A1:D200" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3C4707C1-408B-4B6A-B278-5F3FA8733BBE}" name="RuleID" dataDxfId="15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}" name="Table2" displayName="Table2" ref="A1:G200" totalsRowShown="0">
+  <autoFilter ref="A1:G200" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{3C4707C1-408B-4B6A-B278-5F3FA8733BBE}" name="CORE-ID" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{B88367B4-F155-408A-9DD0-DD0E99F112AE}" name="Version"/>
-    <tableColumn id="2" xr3:uid="{676B4D84-CB39-48B1-86C4-12E66A4FBF76}" name="Message" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{2C710F94-A29A-4635-BD01-2691D10AF83B}" name="Status" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{A6A676A9-AA40-436F-98F7-A4EE26CC9E72}" name="CDISC RuleID"/>
+    <tableColumn id="5" xr3:uid="{7EF9D303-F6DB-4B1F-8692-2CCEB3E74BC2}" name="FDA RuleID"/>
+    <tableColumn id="7" xr3:uid="{FB1FB645-D17D-49C4-96BB-4FA5356E87C4}" name="PMDA RuleID"/>
+    <tableColumn id="2" xr3:uid="{676B4D84-CB39-48B1-86C4-12E66A4FBF76}" name="Message" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{2C710F94-A29A-4635-BD01-2691D10AF83B}" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -773,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D798A9F-8AC0-4EAA-BD02-664438CF629A}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,108 +758,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="8"/>
+      <c r="A1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="7"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>31</v>
+      <c r="A2" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="8"/>
+      <c r="A7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="7"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -893,18 +867,18 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A7:B7"/>
   </mergeCells>
-  <conditionalFormatting sqref="B17:B1048576 A7 B1:B2 B4:B6">
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+  <conditionalFormatting sqref="B17:B1048576 B4:B7 B1:B2">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B16">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -915,10 +889,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C67A62B-6B73-471C-A89D-2B108EA0A071}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,88 +900,84 @@
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.42578125" customWidth="1"/>
     <col min="3" max="3" width="72.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="76.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="76.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
@@ -1188,20 +1158,6 @@
       <c r="C60" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
-      <formula>"notice"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
-      <formula>"warning"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
-      <formula>"Reject"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
-      <formula>"error"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="landscape" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
   <headerFooter>
@@ -1218,15 +1174,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F51C09C-55A4-4B8A-87C6-1EAF95BD08E9}">
   <dimension ref="A1:I150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -1237,31 +1191,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
         <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2017,16 +1971,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"Notice"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"Warning"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>"Reject"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2044,77 +1998,87 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D5F95FA-2C2D-4B1E-A970-B08C9BD5074E}">
-  <dimension ref="A1:D200"/>
+  <dimension ref="A1:G200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="100" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="100" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -2670,11 +2634,11 @@
       <c r="A200" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"SUCCESS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Uses new report template and fixes missing details (#350)
* Uses new report template and fixes missing details

* Add explicit return type for _get_rule_ids
</commit_message>
<xml_diff>
--- a/resources/templates/report-template.xlsx
+++ b/resources/templates/report-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NicHaydel\workspace\cdisc-rules-engine\resources\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bdbelux1-my.sharepoint.com/personal/ndedonder_cro_brussels/Documents/CDISC/CORE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854E8589-3490-4F3A-8B61-AD76AA939DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{BAD70332-1D19-41D1-B6FD-7F9B6B2A0CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F789239-7438-4617-9285-8C33FE2CA11B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{4DEAAD2A-344E-470C-8C9E-CF593FD647F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{4DEAAD2A-344E-470C-8C9E-CF593FD647F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Conformance Details" sheetId="4" r:id="rId1"/>
@@ -37,17 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>Dataset</t>
   </si>
   <si>
-    <t>RuleID</t>
-  </si>
-  <si>
-    <t>Severity</t>
-  </si>
-  <si>
     <t>Explanation</t>
   </si>
   <si>
@@ -111,9 +105,6 @@
     <t>Not configured</t>
   </si>
   <si>
-    <t>Bundle Details</t>
-  </si>
-  <si>
     <t>Define-XML Version</t>
   </si>
   <si>
@@ -132,10 +123,25 @@
     <t>Total Runtime</t>
   </si>
   <si>
+    <t>Executability</t>
+  </si>
+  <si>
+    <t>Standards Details</t>
+  </si>
+  <si>
+    <t>CDISC RuleID</t>
+  </si>
+  <si>
+    <t>FDA RuleID</t>
+  </si>
+  <si>
+    <t>PMDA RuleID</t>
+  </si>
+  <si>
+    <t>CORE-ID</t>
+  </si>
+  <si>
     <t>Data Location</t>
-  </si>
-  <si>
-    <t>Executability</t>
   </si>
 </sst>
 </file>
@@ -187,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -201,9 +207,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -211,7 +214,16 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="21">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -231,98 +243,6 @@
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEDAA00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF40B4E5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEDAA00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF40B4E5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -370,10 +290,62 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDAA00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF40B4E5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -392,8 +364,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="CDISC" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="CDISC" pivot="0" count="2" xr9:uid="{69FBD606-89C9-4CBA-9BEE-430778E41327}">
-      <tableStyleElement type="headerRow" dxfId="24"/>
-      <tableStyleElement type="secondRowStripe" dxfId="23"/>
+      <tableStyleElement type="headerRow" dxfId="20"/>
+      <tableStyleElement type="secondRowStripe" dxfId="19"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -420,17 +392,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{91AB200C-AD87-44CC-B595-CF7F97FFAE49}" name="Table3" displayName="Table3" ref="A1:F60" totalsRowShown="0">
-  <autoFilter ref="A1:F60" xr:uid="{91AB200C-AD87-44CC-B595-CF7F97FFAE49}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{91AB200C-AD87-44CC-B595-CF7F97FFAE49}" name="Table3" displayName="Table3" ref="A1:E60" totalsRowShown="0">
+  <autoFilter ref="A1:E60" xr:uid="{91AB200C-AD87-44CC-B595-CF7F97FFAE49}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
     <sortCondition ref="A2"/>
     <sortCondition ref="B2"/>
   </sortState>
-  <tableColumns count="6">
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{A4677B52-4485-485A-BFC5-88C68D89C965}" name="Dataset"/>
-    <tableColumn id="2" xr3:uid="{FBDFFB0A-6A65-40F7-B7C1-B92B010FBEC9}" name="RuleID" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{3B15064B-7E09-480E-B63C-E93ACA503094}" name="Message" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{F96B2454-B4BC-41CF-97D6-354BF7DA658C}" name="Severity"/>
+    <tableColumn id="2" xr3:uid="{FBDFFB0A-6A65-40F7-B7C1-B92B010FBEC9}" name="CORE-ID" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{3B15064B-7E09-480E-B63C-E93ACA503094}" name="Message" dataDxfId="14"/>
     <tableColumn id="5" xr3:uid="{A33A2D5F-ED56-4ACA-BDB5-A3B54FDFFE4F}" name="Issues"/>
     <tableColumn id="6" xr3:uid="{A33654D2-16F9-4A4C-9ACE-EA3650900336}" name="Explanation"/>
   </tableColumns>
@@ -447,28 +418,31 @@
     <sortCondition ref="E2:E150"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E14C5FBE-76D0-4D41-B4DD-8BBF28D09E06}" name="RuleID" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{36A516EC-8CA6-446B-931B-6DD60430F605}" name="Message" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{E14C5FBE-76D0-4D41-B4DD-8BBF28D09E06}" name="CORE-ID" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{36A516EC-8CA6-446B-931B-6DD60430F605}" name="Message" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{685E7B09-FB5C-4523-8ACB-8B50A8BDD7CB}" name="Executability"/>
     <tableColumn id="4" xr3:uid="{8C809B58-A492-4607-8E72-ED606C841C08}" name="Dataset"/>
     <tableColumn id="5" xr3:uid="{AE7926B7-2872-4A2D-B8DD-CD01A3BC9436}" name="USUBJID"/>
-    <tableColumn id="6" xr3:uid="{0451A533-75C9-49B3-8DDF-A664E805E30A}" name="Record" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{0451A533-75C9-49B3-8DDF-A664E805E30A}" name="Record" dataDxfId="7"/>
     <tableColumn id="7" xr3:uid="{2EC1BE1B-03B8-4035-A6CF-A6F5E7F6ED73}" name="Sequence"/>
-    <tableColumn id="8" xr3:uid="{914E2604-487C-459B-A24D-F233F0858683}" name="Variable(s)" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{19271926-2DDD-4702-94B1-2D701B30975B}" name="Value(s)" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{914E2604-487C-459B-A24D-F233F0858683}" name="Variable(s)" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{19271926-2DDD-4702-94B1-2D701B30975B}" name="Value(s)" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}" name="Table2" displayName="Table2" ref="A1:D200" totalsRowShown="0">
-  <autoFilter ref="A1:D200" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3C4707C1-408B-4B6A-B278-5F3FA8733BBE}" name="RuleID" dataDxfId="15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}" name="Table2" displayName="Table2" ref="A1:G200" totalsRowShown="0">
+  <autoFilter ref="A1:G200" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{3C4707C1-408B-4B6A-B278-5F3FA8733BBE}" name="CORE-ID" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{B88367B4-F155-408A-9DD0-DD0E99F112AE}" name="Version"/>
-    <tableColumn id="2" xr3:uid="{676B4D84-CB39-48B1-86C4-12E66A4FBF76}" name="Message" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{2C710F94-A29A-4635-BD01-2691D10AF83B}" name="Status" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{A6A676A9-AA40-436F-98F7-A4EE26CC9E72}" name="CDISC RuleID"/>
+    <tableColumn id="5" xr3:uid="{7EF9D303-F6DB-4B1F-8692-2CCEB3E74BC2}" name="FDA RuleID"/>
+    <tableColumn id="7" xr3:uid="{FB1FB645-D17D-49C4-96BB-4FA5356E87C4}" name="PMDA RuleID"/>
+    <tableColumn id="2" xr3:uid="{676B4D84-CB39-48B1-86C4-12E66A4FBF76}" name="Message" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{2C710F94-A29A-4635-BD01-2691D10AF83B}" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -773,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D798A9F-8AC0-4EAA-BD02-664438CF629A}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,108 +758,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="8"/>
+      <c r="A1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="7"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>31</v>
+      <c r="A2" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="8"/>
+      <c r="A7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="7"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -893,18 +867,18 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A7:B7"/>
   </mergeCells>
-  <conditionalFormatting sqref="B17:B1048576 A7 B1:B2 B4:B6">
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+  <conditionalFormatting sqref="B17:B1048576 B4:B7 B1:B2">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B16">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -915,10 +889,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C67A62B-6B73-471C-A89D-2B108EA0A071}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,88 +900,84 @@
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.42578125" customWidth="1"/>
     <col min="3" max="3" width="72.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="76.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="76.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
@@ -1188,20 +1158,6 @@
       <c r="C60" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
-      <formula>"notice"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
-      <formula>"warning"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
-      <formula>"Reject"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
-      <formula>"error"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="landscape" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
   <headerFooter>
@@ -1218,15 +1174,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F51C09C-55A4-4B8A-87C6-1EAF95BD08E9}">
   <dimension ref="A1:I150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -1237,31 +1191,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
         <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2017,16 +1971,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"Notice"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"Warning"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>"Reject"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2044,77 +1998,87 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D5F95FA-2C2D-4B1E-A970-B08C9BD5074E}">
-  <dimension ref="A1:D200"/>
+  <dimension ref="A1:G200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="100" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="100" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -2670,11 +2634,11 @@
       <c r="A200" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"SUCCESS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update report template and test reporting issues
</commit_message>
<xml_diff>
--- a/resources/templates/report-template.xlsx
+++ b/resources/templates/report-template.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bdbelux1-my.sharepoint.com/personal/ndedonder_cro_brussels/Documents/CDISC/CORE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{BAD70332-1D19-41D1-B6FD-7F9B6B2A0CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F789239-7438-4617-9285-8C33FE2CA11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{80CEBB2C-D855-4AAF-AA30-61467E87DD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{4DEAAD2A-344E-470C-8C9E-CF593FD647F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Conformance Details" sheetId="4" r:id="rId1"/>
-    <sheet name="Issue Summary" sheetId="1" r:id="rId2"/>
-    <sheet name="Issue Details" sheetId="2" r:id="rId3"/>
-    <sheet name="Rules Report" sheetId="3" r:id="rId4"/>
+    <sheet name="Dataset Details" sheetId="5" r:id="rId2"/>
+    <sheet name="Issue Summary" sheetId="1" r:id="rId3"/>
+    <sheet name="Issue Details" sheetId="2" r:id="rId4"/>
+    <sheet name="Rules Report" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>Dataset</t>
   </si>
@@ -126,6 +127,21 @@
     <t>Executability</t>
   </si>
   <si>
+    <t>CORE Engine Version</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Number of Records</t>
+  </si>
+  <si>
+    <t>Size (kb)</t>
+  </si>
+  <si>
     <t>Standards Details</t>
   </si>
   <si>
@@ -141,7 +157,7 @@
     <t>CORE-ID</t>
   </si>
   <si>
-    <t>Data Location</t>
+    <t>Modified Time Stamp</t>
   </si>
 </sst>
 </file>
@@ -193,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -207,6 +223,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -215,15 +234,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -243,6 +253,67 @@
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDAA00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF40B4E5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -290,62 +361,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEDAA00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF40B4E5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -392,6 +411,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E30721B3-649D-4EEB-BE46-115F06135120}" name="Table4" displayName="Table4" ref="A1:F31" totalsRowShown="0">
+  <autoFilter ref="A1:F31" xr:uid="{E30721B3-649D-4EEB-BE46-115F06135120}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{533FEB42-76B7-4B54-9C62-0B3095066CDB}" name="Dataset"/>
+    <tableColumn id="2" xr3:uid="{A91DF8C0-EBFF-44AA-B85B-6B1988C25C38}" name="Label"/>
+    <tableColumn id="3" xr3:uid="{90E1CEFB-817D-48D1-9A35-A8B9288EC1EC}" name="Location"/>
+    <tableColumn id="6" xr3:uid="{01FFC9E4-1637-4A66-8EE3-DA5E83D12166}" name="Modified Time Stamp"/>
+    <tableColumn id="4" xr3:uid="{CF5555EE-A973-45DC-B63F-6780C4FB6CD9}" name="Size (kb)"/>
+    <tableColumn id="5" xr3:uid="{763786A4-8E65-4277-BBF4-8AEBFB1B12A2}" name="Number of Records"/>
+  </tableColumns>
+  <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{91AB200C-AD87-44CC-B595-CF7F97FFAE49}" name="Table3" displayName="Table3" ref="A1:E60" totalsRowShown="0">
   <autoFilter ref="A1:E60" xr:uid="{91AB200C-AD87-44CC-B595-CF7F97FFAE49}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
@@ -400,8 +434,8 @@
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{A4677B52-4485-485A-BFC5-88C68D89C965}" name="Dataset"/>
-    <tableColumn id="2" xr3:uid="{FBDFFB0A-6A65-40F7-B7C1-B92B010FBEC9}" name="CORE-ID" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{3B15064B-7E09-480E-B63C-E93ACA503094}" name="Message" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{FBDFFB0A-6A65-40F7-B7C1-B92B010FBEC9}" name="CORE-ID" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{3B15064B-7E09-480E-B63C-E93ACA503094}" name="Message" dataDxfId="17"/>
     <tableColumn id="5" xr3:uid="{A33A2D5F-ED56-4ACA-BDB5-A3B54FDFFE4F}" name="Issues"/>
     <tableColumn id="6" xr3:uid="{A33654D2-16F9-4A4C-9ACE-EA3650900336}" name="Explanation"/>
   </tableColumns>
@@ -409,7 +443,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{26759981-A065-432C-A42E-A600CD1C0A1A}" name="Table1" displayName="Table1" ref="A1:I150" totalsRowShown="0">
   <autoFilter ref="A1:I150" xr:uid="{26759981-A065-432C-A42E-A600CD1C0A1A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I150">
@@ -418,31 +452,31 @@
     <sortCondition ref="E2:E150"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E14C5FBE-76D0-4D41-B4DD-8BBF28D09E06}" name="CORE-ID" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{36A516EC-8CA6-446B-931B-6DD60430F605}" name="Message" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{E14C5FBE-76D0-4D41-B4DD-8BBF28D09E06}" name="CORE-ID" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{36A516EC-8CA6-446B-931B-6DD60430F605}" name="Message" dataDxfId="15"/>
     <tableColumn id="3" xr3:uid="{685E7B09-FB5C-4523-8ACB-8B50A8BDD7CB}" name="Executability"/>
     <tableColumn id="4" xr3:uid="{8C809B58-A492-4607-8E72-ED606C841C08}" name="Dataset"/>
     <tableColumn id="5" xr3:uid="{AE7926B7-2872-4A2D-B8DD-CD01A3BC9436}" name="USUBJID"/>
-    <tableColumn id="6" xr3:uid="{0451A533-75C9-49B3-8DDF-A664E805E30A}" name="Record" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{0451A533-75C9-49B3-8DDF-A664E805E30A}" name="Record" dataDxfId="14"/>
     <tableColumn id="7" xr3:uid="{2EC1BE1B-03B8-4035-A6CF-A6F5E7F6ED73}" name="Sequence"/>
-    <tableColumn id="8" xr3:uid="{914E2604-487C-459B-A24D-F233F0858683}" name="Variable(s)" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{19271926-2DDD-4702-94B1-2D701B30975B}" name="Value(s)" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{914E2604-487C-459B-A24D-F233F0858683}" name="Variable(s)" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{19271926-2DDD-4702-94B1-2D701B30975B}" name="Value(s)" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}" name="Table2" displayName="Table2" ref="A1:G200" totalsRowShown="0">
   <autoFilter ref="A1:G200" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3C4707C1-408B-4B6A-B278-5F3FA8733BBE}" name="CORE-ID" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{3C4707C1-408B-4B6A-B278-5F3FA8733BBE}" name="CORE-ID" dataDxfId="11"/>
     <tableColumn id="4" xr3:uid="{B88367B4-F155-408A-9DD0-DD0E99F112AE}" name="Version"/>
     <tableColumn id="6" xr3:uid="{A6A676A9-AA40-436F-98F7-A4EE26CC9E72}" name="CDISC RuleID"/>
     <tableColumn id="5" xr3:uid="{7EF9D303-F6DB-4B1F-8692-2CCEB3E74BC2}" name="FDA RuleID"/>
     <tableColumn id="7" xr3:uid="{FB1FB645-D17D-49C4-96BB-4FA5356E87C4}" name="PMDA RuleID"/>
-    <tableColumn id="2" xr3:uid="{676B4D84-CB39-48B1-86C4-12E66A4FBF76}" name="Message" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{2C710F94-A29A-4635-BD01-2691D10AF83B}" name="Status" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{676B4D84-CB39-48B1-86C4-12E66A4FBF76}" name="Message" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{2C710F94-A29A-4635-BD01-2691D10AF83B}" name="Status" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -745,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D798A9F-8AC0-4EAA-BD02-664438CF629A}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,73 +792,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="8"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>34</v>
+        <v>9</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="8"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="7"/>
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>21</v>
@@ -832,7 +871,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>21</v>
@@ -840,7 +879,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>21</v>
@@ -848,37 +887,29 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="5" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
-  <conditionalFormatting sqref="B17:B1048576 B4:B7 B1:B2">
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+  <conditionalFormatting sqref="B16:B1048576 B1 B3:B6">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8:B16">
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
+  <conditionalFormatting sqref="B7:B15">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+  <conditionalFormatting sqref="B2">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -888,6 +919,52 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FC94AD-F37A-4872-9E7D-6DDF2BAC7C9C}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="3" max="3" width="57.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C67A62B-6B73-471C-A89D-2B108EA0A071}">
   <dimension ref="A1:E60"/>
   <sheetViews>
@@ -909,7 +986,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>25</v>
@@ -1170,7 +1247,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F51C09C-55A4-4B8A-87C6-1EAF95BD08E9}">
   <dimension ref="A1:I150"/>
   <sheetViews>
@@ -1191,7 +1268,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>25</v>
@@ -1971,16 +2048,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Notice"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Warning"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Reject"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1996,7 +2073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D5F95FA-2C2D-4B1E-A970-B08C9BD5074E}">
   <dimension ref="A1:G200"/>
   <sheetViews>
@@ -2015,19 +2092,19 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>25</v>
@@ -2635,10 +2712,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"SUCCESS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update report template and test reporting issues (#358)
* Update report template and test reporting issues

* Update cache

* Convert class to title case to match DETECTABLE_CLASSES

* Apply title casing to excluded classes as well

* Use uppercase class names

* Extract class name conversion method

* Move class name conversion function to utils
</commit_message>
<xml_diff>
--- a/resources/templates/report-template.xlsx
+++ b/resources/templates/report-template.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bdbelux1-my.sharepoint.com/personal/ndedonder_cro_brussels/Documents/CDISC/CORE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{BAD70332-1D19-41D1-B6FD-7F9B6B2A0CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F789239-7438-4617-9285-8C33FE2CA11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{80CEBB2C-D855-4AAF-AA30-61467E87DD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{4DEAAD2A-344E-470C-8C9E-CF593FD647F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Conformance Details" sheetId="4" r:id="rId1"/>
-    <sheet name="Issue Summary" sheetId="1" r:id="rId2"/>
-    <sheet name="Issue Details" sheetId="2" r:id="rId3"/>
-    <sheet name="Rules Report" sheetId="3" r:id="rId4"/>
+    <sheet name="Dataset Details" sheetId="5" r:id="rId2"/>
+    <sheet name="Issue Summary" sheetId="1" r:id="rId3"/>
+    <sheet name="Issue Details" sheetId="2" r:id="rId4"/>
+    <sheet name="Rules Report" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>Dataset</t>
   </si>
@@ -126,6 +127,21 @@
     <t>Executability</t>
   </si>
   <si>
+    <t>CORE Engine Version</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Number of Records</t>
+  </si>
+  <si>
+    <t>Size (kb)</t>
+  </si>
+  <si>
     <t>Standards Details</t>
   </si>
   <si>
@@ -141,7 +157,7 @@
     <t>CORE-ID</t>
   </si>
   <si>
-    <t>Data Location</t>
+    <t>Modified Time Stamp</t>
   </si>
 </sst>
 </file>
@@ -193,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -207,6 +223,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -215,15 +234,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -243,6 +253,67 @@
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDAA00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF40B4E5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -290,62 +361,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEDAA00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF40B4E5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -392,6 +411,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E30721B3-649D-4EEB-BE46-115F06135120}" name="Table4" displayName="Table4" ref="A1:F31" totalsRowShown="0">
+  <autoFilter ref="A1:F31" xr:uid="{E30721B3-649D-4EEB-BE46-115F06135120}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{533FEB42-76B7-4B54-9C62-0B3095066CDB}" name="Dataset"/>
+    <tableColumn id="2" xr3:uid="{A91DF8C0-EBFF-44AA-B85B-6B1988C25C38}" name="Label"/>
+    <tableColumn id="3" xr3:uid="{90E1CEFB-817D-48D1-9A35-A8B9288EC1EC}" name="Location"/>
+    <tableColumn id="6" xr3:uid="{01FFC9E4-1637-4A66-8EE3-DA5E83D12166}" name="Modified Time Stamp"/>
+    <tableColumn id="4" xr3:uid="{CF5555EE-A973-45DC-B63F-6780C4FB6CD9}" name="Size (kb)"/>
+    <tableColumn id="5" xr3:uid="{763786A4-8E65-4277-BBF4-8AEBFB1B12A2}" name="Number of Records"/>
+  </tableColumns>
+  <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{91AB200C-AD87-44CC-B595-CF7F97FFAE49}" name="Table3" displayName="Table3" ref="A1:E60" totalsRowShown="0">
   <autoFilter ref="A1:E60" xr:uid="{91AB200C-AD87-44CC-B595-CF7F97FFAE49}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
@@ -400,8 +434,8 @@
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{A4677B52-4485-485A-BFC5-88C68D89C965}" name="Dataset"/>
-    <tableColumn id="2" xr3:uid="{FBDFFB0A-6A65-40F7-B7C1-B92B010FBEC9}" name="CORE-ID" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{3B15064B-7E09-480E-B63C-E93ACA503094}" name="Message" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{FBDFFB0A-6A65-40F7-B7C1-B92B010FBEC9}" name="CORE-ID" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{3B15064B-7E09-480E-B63C-E93ACA503094}" name="Message" dataDxfId="17"/>
     <tableColumn id="5" xr3:uid="{A33A2D5F-ED56-4ACA-BDB5-A3B54FDFFE4F}" name="Issues"/>
     <tableColumn id="6" xr3:uid="{A33654D2-16F9-4A4C-9ACE-EA3650900336}" name="Explanation"/>
   </tableColumns>
@@ -409,7 +443,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{26759981-A065-432C-A42E-A600CD1C0A1A}" name="Table1" displayName="Table1" ref="A1:I150" totalsRowShown="0">
   <autoFilter ref="A1:I150" xr:uid="{26759981-A065-432C-A42E-A600CD1C0A1A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I150">
@@ -418,31 +452,31 @@
     <sortCondition ref="E2:E150"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E14C5FBE-76D0-4D41-B4DD-8BBF28D09E06}" name="CORE-ID" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{36A516EC-8CA6-446B-931B-6DD60430F605}" name="Message" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{E14C5FBE-76D0-4D41-B4DD-8BBF28D09E06}" name="CORE-ID" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{36A516EC-8CA6-446B-931B-6DD60430F605}" name="Message" dataDxfId="15"/>
     <tableColumn id="3" xr3:uid="{685E7B09-FB5C-4523-8ACB-8B50A8BDD7CB}" name="Executability"/>
     <tableColumn id="4" xr3:uid="{8C809B58-A492-4607-8E72-ED606C841C08}" name="Dataset"/>
     <tableColumn id="5" xr3:uid="{AE7926B7-2872-4A2D-B8DD-CD01A3BC9436}" name="USUBJID"/>
-    <tableColumn id="6" xr3:uid="{0451A533-75C9-49B3-8DDF-A664E805E30A}" name="Record" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{0451A533-75C9-49B3-8DDF-A664E805E30A}" name="Record" dataDxfId="14"/>
     <tableColumn id="7" xr3:uid="{2EC1BE1B-03B8-4035-A6CF-A6F5E7F6ED73}" name="Sequence"/>
-    <tableColumn id="8" xr3:uid="{914E2604-487C-459B-A24D-F233F0858683}" name="Variable(s)" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{19271926-2DDD-4702-94B1-2D701B30975B}" name="Value(s)" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{914E2604-487C-459B-A24D-F233F0858683}" name="Variable(s)" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{19271926-2DDD-4702-94B1-2D701B30975B}" name="Value(s)" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}" name="Table2" displayName="Table2" ref="A1:G200" totalsRowShown="0">
   <autoFilter ref="A1:G200" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3C4707C1-408B-4B6A-B278-5F3FA8733BBE}" name="CORE-ID" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{3C4707C1-408B-4B6A-B278-5F3FA8733BBE}" name="CORE-ID" dataDxfId="11"/>
     <tableColumn id="4" xr3:uid="{B88367B4-F155-408A-9DD0-DD0E99F112AE}" name="Version"/>
     <tableColumn id="6" xr3:uid="{A6A676A9-AA40-436F-98F7-A4EE26CC9E72}" name="CDISC RuleID"/>
     <tableColumn id="5" xr3:uid="{7EF9D303-F6DB-4B1F-8692-2CCEB3E74BC2}" name="FDA RuleID"/>
     <tableColumn id="7" xr3:uid="{FB1FB645-D17D-49C4-96BB-4FA5356E87C4}" name="PMDA RuleID"/>
-    <tableColumn id="2" xr3:uid="{676B4D84-CB39-48B1-86C4-12E66A4FBF76}" name="Message" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{2C710F94-A29A-4635-BD01-2691D10AF83B}" name="Status" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{676B4D84-CB39-48B1-86C4-12E66A4FBF76}" name="Message" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{2C710F94-A29A-4635-BD01-2691D10AF83B}" name="Status" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -745,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D798A9F-8AC0-4EAA-BD02-664438CF629A}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,73 +792,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="8"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>34</v>
+        <v>9</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="8"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="7"/>
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>21</v>
@@ -832,7 +871,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>21</v>
@@ -840,7 +879,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>21</v>
@@ -848,37 +887,29 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="5" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
-  <conditionalFormatting sqref="B17:B1048576 B4:B7 B1:B2">
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+  <conditionalFormatting sqref="B16:B1048576 B1 B3:B6">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8:B16">
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
+  <conditionalFormatting sqref="B7:B15">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+  <conditionalFormatting sqref="B2">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -888,6 +919,52 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FC94AD-F37A-4872-9E7D-6DDF2BAC7C9C}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="3" max="3" width="57.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C67A62B-6B73-471C-A89D-2B108EA0A071}">
   <dimension ref="A1:E60"/>
   <sheetViews>
@@ -909,7 +986,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>25</v>
@@ -1170,7 +1247,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F51C09C-55A4-4B8A-87C6-1EAF95BD08E9}">
   <dimension ref="A1:I150"/>
   <sheetViews>
@@ -1191,7 +1268,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>25</v>
@@ -1971,16 +2048,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Notice"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Warning"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Reject"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1996,7 +2073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D5F95FA-2C2D-4B1E-A970-B08C9BD5074E}">
   <dimension ref="A1:G200"/>
   <sheetViews>
@@ -2015,19 +2092,19 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>25</v>
@@ -2635,10 +2712,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"SUCCESS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Report on "ISSUE_REPORTED" and "EXECUTION_ERROR"
</commit_message>
<xml_diff>
--- a/resources/templates/report-template.xlsx
+++ b/resources/templates/report-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bdbelux1-my.sharepoint.com/personal/ndedonder_cro_brussels/Documents/CDISC/CORE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GerryCampion\Code\cdisc-rules-engine\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80CEBB2C-D855-4AAF-AA30-61467E87DD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F90ACC-D4D4-42AD-B33D-8703DEE58190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{4DEAAD2A-344E-470C-8C9E-CF593FD647F4}"/>
+    <workbookView xWindow="5460" yWindow="1935" windowWidth="26475" windowHeight="17370" xr2:uid="{4DEAAD2A-344E-470C-8C9E-CF593FD647F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Conformance Details" sheetId="4" r:id="rId1"/>
@@ -233,7 +233,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDAA00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -282,20 +322,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF40B4E5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
         </patternFill>
       </fill>
     </dxf>
@@ -383,8 +409,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="CDISC" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="CDISC" pivot="0" count="2" xr9:uid="{69FBD606-89C9-4CBA-9BEE-430778E41327}">
-      <tableStyleElement type="headerRow" dxfId="20"/>
-      <tableStyleElement type="secondRowStripe" dxfId="19"/>
+      <tableStyleElement type="headerRow" dxfId="22"/>
+      <tableStyleElement type="secondRowStripe" dxfId="21"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -434,8 +460,8 @@
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{A4677B52-4485-485A-BFC5-88C68D89C965}" name="Dataset"/>
-    <tableColumn id="2" xr3:uid="{FBDFFB0A-6A65-40F7-B7C1-B92B010FBEC9}" name="CORE-ID" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{3B15064B-7E09-480E-B63C-E93ACA503094}" name="Message" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{FBDFFB0A-6A65-40F7-B7C1-B92B010FBEC9}" name="CORE-ID" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{3B15064B-7E09-480E-B63C-E93ACA503094}" name="Message" dataDxfId="19"/>
     <tableColumn id="5" xr3:uid="{A33A2D5F-ED56-4ACA-BDB5-A3B54FDFFE4F}" name="Issues"/>
     <tableColumn id="6" xr3:uid="{A33654D2-16F9-4A4C-9ACE-EA3650900336}" name="Explanation"/>
   </tableColumns>
@@ -452,31 +478,31 @@
     <sortCondition ref="E2:E150"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E14C5FBE-76D0-4D41-B4DD-8BBF28D09E06}" name="CORE-ID" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{36A516EC-8CA6-446B-931B-6DD60430F605}" name="Message" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{E14C5FBE-76D0-4D41-B4DD-8BBF28D09E06}" name="CORE-ID" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{36A516EC-8CA6-446B-931B-6DD60430F605}" name="Message" dataDxfId="17"/>
     <tableColumn id="3" xr3:uid="{685E7B09-FB5C-4523-8ACB-8B50A8BDD7CB}" name="Executability"/>
     <tableColumn id="4" xr3:uid="{8C809B58-A492-4607-8E72-ED606C841C08}" name="Dataset"/>
     <tableColumn id="5" xr3:uid="{AE7926B7-2872-4A2D-B8DD-CD01A3BC9436}" name="USUBJID"/>
-    <tableColumn id="6" xr3:uid="{0451A533-75C9-49B3-8DDF-A664E805E30A}" name="Record" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{0451A533-75C9-49B3-8DDF-A664E805E30A}" name="Record" dataDxfId="16"/>
     <tableColumn id="7" xr3:uid="{2EC1BE1B-03B8-4035-A6CF-A6F5E7F6ED73}" name="Sequence"/>
-    <tableColumn id="8" xr3:uid="{914E2604-487C-459B-A24D-F233F0858683}" name="Variable(s)" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{19271926-2DDD-4702-94B1-2D701B30975B}" name="Value(s)" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{914E2604-487C-459B-A24D-F233F0858683}" name="Variable(s)" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{19271926-2DDD-4702-94B1-2D701B30975B}" name="Value(s)" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}" name="Table2" displayName="Table2" ref="A1:G200" totalsRowShown="0">
-  <autoFilter ref="A1:G200" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}" name="Table2" displayName="Table2" ref="A1:G501" totalsRowShown="0">
+  <autoFilter ref="A1:G501" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3C4707C1-408B-4B6A-B278-5F3FA8733BBE}" name="CORE-ID" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{3C4707C1-408B-4B6A-B278-5F3FA8733BBE}" name="CORE-ID" dataDxfId="13"/>
     <tableColumn id="4" xr3:uid="{B88367B4-F155-408A-9DD0-DD0E99F112AE}" name="Version"/>
     <tableColumn id="6" xr3:uid="{A6A676A9-AA40-436F-98F7-A4EE26CC9E72}" name="CDISC RuleID"/>
     <tableColumn id="5" xr3:uid="{7EF9D303-F6DB-4B1F-8692-2CCEB3E74BC2}" name="FDA RuleID"/>
     <tableColumn id="7" xr3:uid="{FB1FB645-D17D-49C4-96BB-4FA5356E87C4}" name="PMDA RuleID"/>
-    <tableColumn id="2" xr3:uid="{676B4D84-CB39-48B1-86C4-12E66A4FBF76}" name="Message" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{2C710F94-A29A-4635-BD01-2691D10AF83B}" name="Status" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{676B4D84-CB39-48B1-86C4-12E66A4FBF76}" name="Message" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{2C710F94-A29A-4635-BD01-2691D10AF83B}" name="Status" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -898,18 +924,8 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A6:B6"/>
   </mergeCells>
-  <conditionalFormatting sqref="B16:B1048576 B1 B3:B6">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
-      <formula>"not configured"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7:B15">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
-      <formula>"not configured"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2048,16 +2064,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"Notice"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"Warning"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"Reject"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2075,7 +2091,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D5F95FA-2C2D-4B1E-A970-B08C9BD5074E}">
-  <dimension ref="A1:G200"/>
+  <dimension ref="A1:G501"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2710,13 +2726,922 @@
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
     </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="1"/>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="1"/>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="1"/>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="1"/>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="1"/>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="1"/>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="1"/>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="1"/>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="1"/>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="1"/>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="1"/>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="1"/>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="1"/>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="1"/>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="1"/>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="1"/>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="1"/>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="1"/>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" s="1"/>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="1"/>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="1"/>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="1"/>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" s="1"/>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="1"/>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="1"/>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="1"/>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="1"/>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="1"/>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="1"/>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="1"/>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="1"/>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="1"/>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="1"/>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="1"/>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="1"/>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="1"/>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="1"/>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" s="1"/>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" s="1"/>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" s="1"/>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" s="1"/>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" s="1"/>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" s="1"/>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" s="1"/>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" s="1"/>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" s="1"/>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" s="1"/>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" s="1"/>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" s="1"/>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" s="1"/>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" s="1"/>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" s="1"/>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" s="1"/>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" s="1"/>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" s="1"/>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" s="1"/>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" s="1"/>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" s="1"/>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" s="1"/>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" s="1"/>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" s="1"/>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" s="1"/>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" s="1"/>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" s="1"/>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" s="1"/>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" s="1"/>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" s="1"/>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" s="1"/>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" s="1"/>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" s="1"/>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" s="1"/>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" s="1"/>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" s="1"/>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" s="1"/>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" s="1"/>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" s="1"/>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" s="1"/>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" s="1"/>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" s="1"/>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" s="1"/>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281" s="1"/>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282" s="1"/>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" s="1"/>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" s="1"/>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" s="1"/>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" s="1"/>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" s="1"/>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" s="1"/>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" s="1"/>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" s="1"/>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" s="1"/>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" s="1"/>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" s="1"/>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" s="1"/>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" s="1"/>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" s="1"/>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" s="1"/>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298" s="1"/>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299" s="1"/>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" s="1"/>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" s="1"/>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" s="1"/>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303" s="1"/>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304" s="1"/>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305" s="1"/>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" s="1"/>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" s="1"/>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" s="1"/>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" s="1"/>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" s="1"/>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311" s="1"/>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" s="1"/>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" s="1"/>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A314" s="1"/>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A315" s="1"/>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A316" s="1"/>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A317" s="1"/>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A318" s="1"/>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A319" s="1"/>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A320" s="1"/>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A321" s="1"/>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A322" s="1"/>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A323" s="1"/>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A324" s="1"/>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A325" s="1"/>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A326" s="1"/>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A327" s="1"/>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A328" s="1"/>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A329" s="1"/>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A330" s="1"/>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A331" s="1"/>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A332" s="1"/>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A333" s="1"/>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A334" s="1"/>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A335" s="1"/>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A336" s="1"/>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337" s="1"/>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338" s="1"/>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A339" s="1"/>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A340" s="1"/>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A341" s="1"/>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A342" s="1"/>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A343" s="1"/>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A344" s="1"/>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A345" s="1"/>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A346" s="1"/>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A347" s="1"/>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A348" s="1"/>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A349" s="1"/>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A350" s="1"/>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A351" s="1"/>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A352" s="1"/>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A353" s="1"/>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A354" s="1"/>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A355" s="1"/>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A356" s="1"/>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A357" s="1"/>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A358" s="1"/>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A359" s="1"/>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" s="1"/>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361" s="1"/>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362" s="1"/>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363" s="1"/>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" s="1"/>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365" s="1"/>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" s="1"/>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" s="1"/>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" s="1"/>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" s="1"/>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" s="1"/>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" s="1"/>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" s="1"/>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" s="1"/>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" s="1"/>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" s="1"/>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" s="1"/>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" s="1"/>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" s="1"/>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" s="1"/>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380" s="1"/>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381" s="1"/>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" s="1"/>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" s="1"/>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" s="1"/>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" s="1"/>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" s="1"/>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" s="1"/>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" s="1"/>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" s="1"/>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" s="1"/>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391" s="1"/>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392" s="1"/>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A393" s="1"/>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A394" s="1"/>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A395" s="1"/>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A396" s="1"/>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A397" s="1"/>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A398" s="1"/>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A399" s="1"/>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A400" s="1"/>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A401" s="1"/>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A402" s="1"/>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403" s="1"/>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404" s="1"/>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" s="1"/>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" s="1"/>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" s="1"/>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" s="1"/>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" s="1"/>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" s="1"/>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" s="1"/>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" s="1"/>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" s="1"/>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" s="1"/>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" s="1"/>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" s="1"/>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" s="1"/>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" s="1"/>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" s="1"/>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" s="1"/>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" s="1"/>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" s="1"/>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" s="1"/>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" s="1"/>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" s="1"/>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" s="1"/>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" s="1"/>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428" s="1"/>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429" s="1"/>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" s="1"/>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" s="1"/>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432" s="1"/>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A433" s="1"/>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A434" s="1"/>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A435" s="1"/>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A436" s="1"/>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A437" s="1"/>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A438" s="1"/>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A439" s="1"/>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A440" s="1"/>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A441" s="1"/>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A442" s="1"/>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A443" s="1"/>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444" s="1"/>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445" s="1"/>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446" s="1"/>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447" s="1"/>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A448" s="1"/>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449" s="1"/>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450" s="1"/>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A451" s="1"/>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A452" s="1"/>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A453" s="1"/>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A454" s="1"/>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A455" s="1"/>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A456" s="1"/>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A457" s="1"/>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A458" s="1"/>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A459" s="1"/>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A460" s="1"/>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A461" s="1"/>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A462" s="1"/>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A463" s="1"/>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A464" s="1"/>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A465" s="1"/>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A466" s="1"/>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A467" s="1"/>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A468" s="1"/>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A469" s="1"/>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A470" s="1"/>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A471" s="1"/>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A472" s="1"/>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A473" s="1"/>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A474" s="1"/>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A475" s="1"/>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A476" s="1"/>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A477" s="1"/>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478" s="1"/>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A479" s="1"/>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A480" s="1"/>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A481" s="1"/>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A482" s="1"/>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A483" s="1"/>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A484" s="1"/>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A485" s="1"/>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A486" s="1"/>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A487" s="1"/>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A488" s="1"/>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A489" s="1"/>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A490" s="1"/>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A491" s="1"/>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A492" s="1"/>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A493" s="1"/>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A494" s="1"/>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A495" s="1"/>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A496" s="1"/>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A497" s="1"/>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A498" s="1"/>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A499" s="1"/>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A500" s="1"/>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A501" s="1"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"SUCCESS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>"ISSUE_REPORTED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"SKIPPED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"EXECUTION_ERROR"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated report template, getting domain into report
</commit_message>
<xml_diff>
--- a/resources/templates/report-template.xlsx
+++ b/resources/templates/report-template.xlsx
@@ -1,51 +1,112 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bdbelux1-my.sharepoint.com/personal/ndedonder_cro_brussels/Documents/CDISC/CORE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SamJohnson\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80CEBB2C-D855-4AAF-AA30-61467E87DD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{861A05AC-7E66-4324-829A-83AC6D292316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{4DEAAD2A-344E-470C-8C9E-CF593FD647F4}"/>
+    <workbookView xWindow="14805" yWindow="1050" windowWidth="29400" windowHeight="19305" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Conformance Details" sheetId="4" r:id="rId1"/>
-    <sheet name="Dataset Details" sheetId="5" r:id="rId2"/>
-    <sheet name="Issue Summary" sheetId="1" r:id="rId3"/>
-    <sheet name="Issue Details" sheetId="2" r:id="rId4"/>
-    <sheet name="Rules Report" sheetId="3" r:id="rId5"/>
+    <sheet name="Conformance Details" sheetId="1" r:id="rId1"/>
+    <sheet name="Dataset Details" sheetId="2" r:id="rId2"/>
+    <sheet name="Issue Summary" sheetId="3" r:id="rId3"/>
+    <sheet name="Issue Details" sheetId="4" r:id="rId4"/>
+    <sheet name="Rules Report" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+  <si>
+    <t>Conformance Details</t>
+  </si>
+  <si>
+    <t>Report Generation</t>
+  </si>
+  <si>
+    <t>Total Runtime</t>
+  </si>
+  <si>
+    <t>CORE Engine Version</t>
+  </si>
+  <si>
+    <t>Standards Details</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>CT Version</t>
+  </si>
+  <si>
+    <t>Define-XML Version</t>
+  </si>
+  <si>
+    <t>UNII Version</t>
+  </si>
+  <si>
+    <t>Med-RT Version</t>
+  </si>
+  <si>
+    <t>MedDRA Version</t>
+  </si>
+  <si>
+    <t>WHODRUG Version</t>
+  </si>
+  <si>
+    <t>SNOMED Version</t>
+  </si>
   <si>
     <t>Dataset</t>
   </si>
   <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Modified Time Stamp</t>
+  </si>
+  <si>
+    <t>Size (kb)</t>
+  </si>
+  <si>
+    <t>Number of Records</t>
+  </si>
+  <si>
+    <t>CORE-ID</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Issues</t>
+  </si>
+  <si>
     <t>Explanation</t>
   </si>
   <si>
+    <t>CORE-000334</t>
+  </si>
+  <si>
+    <t>At least one expected variable is missing from dataset</t>
+  </si>
+  <si>
+    <t>Executability</t>
+  </si>
+  <si>
     <t>USUBJID</t>
   </si>
   <si>
@@ -61,103 +122,28 @@
     <t>Value(s)</t>
   </si>
   <si>
-    <t>Issues</t>
-  </si>
-  <si>
-    <t>Conformance Details</t>
-  </si>
-  <si>
-    <t>Report Generation</t>
-  </si>
-  <si>
-    <t>Standard</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>CT Version</t>
-  </si>
-  <si>
-    <t>UNII Version</t>
-  </si>
-  <si>
-    <t>Med-RT Version</t>
-  </si>
-  <si>
-    <t>MedDRA Version</t>
-  </si>
-  <si>
-    <t>WHODRUG Version</t>
-  </si>
-  <si>
-    <t>SDTM</t>
-  </si>
-  <si>
-    <t>2021-11-24T10:50:24</t>
-  </si>
-  <si>
-    <t>V3.4</t>
-  </si>
-  <si>
-    <t>2021-09-24</t>
-  </si>
-  <si>
-    <t>Not configured</t>
-  </si>
-  <si>
-    <t>Define-XML Version</t>
-  </si>
-  <si>
-    <t>2.1</t>
-  </si>
-  <si>
-    <t>SNOMED Version</t>
-  </si>
-  <si>
-    <t>Message</t>
+    <t>CDISC RuleID</t>
+  </si>
+  <si>
+    <t>FDA RuleID</t>
+  </si>
+  <si>
+    <t>PMDA RuleID</t>
   </si>
   <si>
     <t>Status</t>
   </si>
   <si>
-    <t>Total Runtime</t>
-  </si>
-  <si>
-    <t>Executability</t>
-  </si>
-  <si>
-    <t>CORE Engine Version</t>
-  </si>
-  <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Number of Records</t>
-  </si>
-  <si>
-    <t>Size (kb)</t>
-  </si>
-  <si>
-    <t>Standards Details</t>
-  </si>
-  <si>
-    <t>CDISC RuleID</t>
-  </si>
-  <si>
-    <t>FDA RuleID</t>
-  </si>
-  <si>
-    <t>PMDA RuleID</t>
-  </si>
-  <si>
-    <t>CORE-ID</t>
-  </si>
-  <si>
-    <t>Modified Time Stamp</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>CG0016</t>
+  </si>
+  <si>
+    <t>SUCCESS</t>
+  </si>
+  <si>
+    <t>Dataset Domain</t>
   </si>
 </sst>
 </file>
@@ -209,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -229,11 +215,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="19">
     <dxf>
       <font>
         <color auto="1"/>
@@ -293,78 +280,56 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
     </dxf>
     <dxf>
       <fill>
@@ -382,23 +347,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="CDISC" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="CDISC" pivot="0" count="2" xr9:uid="{69FBD606-89C9-4CBA-9BEE-430778E41327}">
-      <tableStyleElement type="headerRow" dxfId="20"/>
-      <tableStyleElement type="secondRowStripe" dxfId="19"/>
+    <tableStyle name="CDISC" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="18"/>
+      <tableStyleElement type="secondRowStripe" dxfId="17"/>
     </tableStyle>
   </tableStyles>
-  <colors>
-    <mruColors>
-      <color rgb="FFEDAA00"/>
-      <color rgb="FFC94543"/>
-      <color rgb="FFA1D0CA"/>
-      <color rgb="FF40B4E5"/>
-      <color rgb="FFCCE6E3"/>
-      <color rgb="FFFFFF66"/>
-      <color rgb="FFFF7C80"/>
-      <color rgb="FFFF3300"/>
-    </mruColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -411,72 +364,74 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E30721B3-649D-4EEB-BE46-115F06135120}" name="Table4" displayName="Table4" ref="A1:F31" totalsRowShown="0">
-  <autoFilter ref="A1:F31" xr:uid="{E30721B3-649D-4EEB-BE46-115F06135120}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table4" displayName="Table4" ref="A1:F31" totalsRowShown="0">
+  <autoFilter ref="A1:F31" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{533FEB42-76B7-4B54-9C62-0B3095066CDB}" name="Dataset"/>
-    <tableColumn id="2" xr3:uid="{A91DF8C0-EBFF-44AA-B85B-6B1988C25C38}" name="Label"/>
-    <tableColumn id="3" xr3:uid="{90E1CEFB-817D-48D1-9A35-A8B9288EC1EC}" name="Location"/>
-    <tableColumn id="6" xr3:uid="{01FFC9E4-1637-4A66-8EE3-DA5E83D12166}" name="Modified Time Stamp"/>
-    <tableColumn id="4" xr3:uid="{CF5555EE-A973-45DC-B63F-6780C4FB6CD9}" name="Size (kb)"/>
-    <tableColumn id="5" xr3:uid="{763786A4-8E65-4277-BBF4-8AEBFB1B12A2}" name="Number of Records"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Dataset"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Label"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Location"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Modified Time Stamp"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Size (kb)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Number of Records"/>
   </tableColumns>
   <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{91AB200C-AD87-44CC-B595-CF7F97FFAE49}" name="Table3" displayName="Table3" ref="A1:E60" totalsRowShown="0">
-  <autoFilter ref="A1:E60" xr:uid="{91AB200C-AD87-44CC-B595-CF7F97FFAE49}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E2">
-    <sortCondition ref="A2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="A1:F60" totalsRowShown="0">
+  <autoFilter ref="A1:F60" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:F2">
     <sortCondition ref="B2"/>
+    <sortCondition ref="C2"/>
   </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A4677B52-4485-485A-BFC5-88C68D89C965}" name="Dataset"/>
-    <tableColumn id="2" xr3:uid="{FBDFFB0A-6A65-40F7-B7C1-B92B010FBEC9}" name="CORE-ID" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{3B15064B-7E09-480E-B63C-E93ACA503094}" name="Message" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{A33A2D5F-ED56-4ACA-BDB5-A3B54FDFFE4F}" name="Issues"/>
-    <tableColumn id="6" xr3:uid="{A33654D2-16F9-4A4C-9ACE-EA3650900336}" name="Explanation"/>
+  <tableColumns count="6">
+    <tableColumn id="4" xr3:uid="{4CBF66AF-B6BA-435A-B965-53A8B1955465}" name="Dataset"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Dataset Domain"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="CORE-ID" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Message" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Issues"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Explanation"/>
   </tableColumns>
   <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{26759981-A065-432C-A42E-A600CD1C0A1A}" name="Table1" displayName="Table1" ref="A1:I150" totalsRowShown="0">
-  <autoFilter ref="A1:I150" xr:uid="{26759981-A065-432C-A42E-A600CD1C0A1A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I150">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table1" displayName="Table1" ref="A1:J150" totalsRowShown="0">
+  <autoFilter ref="A1:J150" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J150">
     <sortCondition ref="A2:A150"/>
-    <sortCondition ref="D2:D150"/>
     <sortCondition ref="E2:E150"/>
+    <sortCondition ref="F2:F150"/>
   </sortState>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E14C5FBE-76D0-4D41-B4DD-8BBF28D09E06}" name="CORE-ID" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{36A516EC-8CA6-446B-931B-6DD60430F605}" name="Message" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{685E7B09-FB5C-4523-8ACB-8B50A8BDD7CB}" name="Executability"/>
-    <tableColumn id="4" xr3:uid="{8C809B58-A492-4607-8E72-ED606C841C08}" name="Dataset"/>
-    <tableColumn id="5" xr3:uid="{AE7926B7-2872-4A2D-B8DD-CD01A3BC9436}" name="USUBJID"/>
-    <tableColumn id="6" xr3:uid="{0451A533-75C9-49B3-8DDF-A664E805E30A}" name="Record" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{2EC1BE1B-03B8-4035-A6CF-A6F5E7F6ED73}" name="Sequence"/>
-    <tableColumn id="8" xr3:uid="{914E2604-487C-459B-A24D-F233F0858683}" name="Variable(s)" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{19271926-2DDD-4702-94B1-2D701B30975B}" name="Value(s)" dataDxfId="12"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="CORE-ID" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Message" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Executability"/>
+    <tableColumn id="10" xr3:uid="{9C910915-7F0C-466C-85EF-3D81E52EA236}" name="Dataset"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Dataset Domain"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="USUBJID"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Record" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Sequence"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Variable(s)" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Value(s)" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}" name="Table2" displayName="Table2" ref="A1:G200" totalsRowShown="0">
-  <autoFilter ref="A1:G200" xr:uid="{13EEEF43-0886-4B7E-9FAA-532F41C914FA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table2" displayName="Table2" ref="A1:G200" totalsRowShown="0">
+  <autoFilter ref="A1:G200" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3C4707C1-408B-4B6A-B278-5F3FA8733BBE}" name="CORE-ID" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{B88367B4-F155-408A-9DD0-DD0E99F112AE}" name="Version"/>
-    <tableColumn id="6" xr3:uid="{A6A676A9-AA40-436F-98F7-A4EE26CC9E72}" name="CDISC RuleID"/>
-    <tableColumn id="5" xr3:uid="{7EF9D303-F6DB-4B1F-8692-2CCEB3E74BC2}" name="FDA RuleID"/>
-    <tableColumn id="7" xr3:uid="{FB1FB645-D17D-49C4-96BB-4FA5356E87C4}" name="PMDA RuleID"/>
-    <tableColumn id="2" xr3:uid="{676B4D84-CB39-48B1-86C4-12E66A4FBF76}" name="Message" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{2C710F94-A29A-4635-BD01-2691D10AF83B}" name="Status" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="CORE-ID" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Version"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="CDISC RuleID"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="FDA RuleID"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="PMDA RuleID"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Message" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Status" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -778,11 +733,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D798A9F-8AC0-4EAA-BD02-664438CF629A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,104 +748,78 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>27</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B3"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>29</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B4"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="8"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="9"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>20</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B9" s="6"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>23</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B10" s="6"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -898,32 +827,22 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A6:B6"/>
   </mergeCells>
-  <conditionalFormatting sqref="B16:B1048576 B1 B3:B6">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
-      <formula>"not configured"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7:B15">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
-      <formula>"not configured"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
+  <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FC94AD-F37A-4872-9E7D-6DDF2BAC7C9C}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,23 +857,247 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>32</v>
-      </c>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -965,1089 +1108,1119 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C67A62B-6B73-471C-A89D-2B108EA0A071}">
-  <dimension ref="A1:E60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="72.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="76.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="66" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="65.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="1"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="1"/>
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="1"/>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="1"/>
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="1"/>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="1"/>
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="1"/>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="1"/>
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="1"/>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="1"/>
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="1"/>
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C43" s="1"/>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="1"/>
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C44" s="1"/>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="1"/>
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="1"/>
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C46" s="1"/>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="1"/>
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C47" s="1"/>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="1"/>
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C48" s="1"/>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="1"/>
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C49" s="1"/>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="1"/>
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C50" s="1"/>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="1"/>
+      <c r="D50" s="1"/>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C51" s="1"/>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="1"/>
+      <c r="D51" s="1"/>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C52" s="1"/>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="1"/>
+      <c r="D52" s="1"/>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C53" s="1"/>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="1"/>
+      <c r="D53" s="1"/>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C54" s="1"/>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="1"/>
+      <c r="D54" s="1"/>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C55" s="1"/>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="1"/>
+      <c r="D55" s="1"/>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C56" s="1"/>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="1"/>
+      <c r="D56" s="1"/>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C57" s="1"/>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="1"/>
+      <c r="D57" s="1"/>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C58" s="1"/>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="1"/>
+      <c r="D58" s="1"/>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C59" s="1"/>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="1"/>
+      <c r="D59" s="1"/>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup orientation="landscape" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125978" footer="0.31496062992125978"/>
+  <pageSetup orientation="landscape" horizontalDpi="90" verticalDpi="90"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;G</oddHeader>
   </headerFooter>
-  <legacyDrawingHF r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F51C09C-55A4-4B8A-87C6-1EAF95BD08E9}">
-  <dimension ref="A1:I150"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:K150"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="64.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="59.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="64.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
+      <c r="H1" t="s">
+        <v>29</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="1"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G4" s="2"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G5" s="2"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G6" s="2"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G7" s="2"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G8" s="2"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G9" s="2"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G10" s="2"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
-      <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
-      <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
-      <c r="F38" s="2"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
-      <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
-      <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
-      <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
-      <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
-      <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
-      <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
-      <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
-      <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
-      <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
-      <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48" s="2"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
-      <c r="F49" s="2"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" s="2"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
-      <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" s="2"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
-      <c r="F51" s="2"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51" s="2"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
-      <c r="F52" s="2"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52" s="2"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
-      <c r="F53" s="2"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53" s="2"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
-      <c r="F54" s="2"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54" s="2"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
-      <c r="F55" s="2"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55" s="2"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
-      <c r="F56" s="2"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56" s="2"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
-      <c r="F57" s="2"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57" s="2"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
-      <c r="F58" s="2"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58" s="2"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
-      <c r="F59" s="2"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59" s="2"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
-      <c r="F60" s="2"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G60" s="2"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
-      <c r="F61" s="2"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61" s="2"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
-      <c r="F62" s="2"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G62" s="2"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
-      <c r="F63" s="2"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63" s="2"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
-      <c r="F64" s="2"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G64" s="2"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
-      <c r="F65" s="2"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G65" s="2"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
-      <c r="F66" s="2"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G66" s="2"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
-      <c r="F67" s="2"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G67" s="2"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
-      <c r="F68" s="2"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G68" s="2"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
-      <c r="F69" s="2"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G69" s="2"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
-      <c r="F70" s="2"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G70" s="2"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
-      <c r="F71" s="2"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G71" s="2"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
-      <c r="F72" s="2"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G72" s="2"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
-      <c r="F73" s="2"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G73" s="2"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
-      <c r="F74" s="2"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G74" s="2"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
-      <c r="F75" s="2"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G75" s="2"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
-      <c r="F76" s="2"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G76" s="2"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="2"/>
-      <c r="F77" s="2"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G77" s="2"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
-      <c r="F78" s="2"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G78" s="2"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
-      <c r="F79" s="2"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G79" s="2"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
-      <c r="F80" s="2"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G80" s="2"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="2"/>
-      <c r="F81" s="2"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G81" s="2"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="2"/>
-      <c r="F82" s="2"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G82" s="2"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
-      <c r="F83" s="2"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G83" s="2"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
-      <c r="F84" s="2"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G84" s="2"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
-      <c r="F85" s="2"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G85" s="2"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
-      <c r="F86" s="2"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G86" s="2"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
-      <c r="F87" s="2"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G87" s="2"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
-      <c r="F88" s="2"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G88" s="2"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
-      <c r="F89" s="2"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G89" s="2"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
-      <c r="F90" s="2"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G90" s="2"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
-      <c r="F91" s="2"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G91" s="2"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
-      <c r="F92" s="2"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G92" s="2"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
-      <c r="F93" s="2"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G93" s="2"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
-      <c r="F94" s="2"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G94" s="2"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
-      <c r="F95" s="2"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G95" s="2"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
-      <c r="F96" s="2"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G96" s="2"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
-      <c r="F97" s="2"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G97" s="2"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="2"/>
-      <c r="F98" s="2"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G98" s="2"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="2"/>
-      <c r="F99" s="2"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G99" s="2"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="2"/>
-      <c r="F100" s="2"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G100" s="2"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="2"/>
-      <c r="F101" s="2"/>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G101" s="2"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="2"/>
-      <c r="F102" s="2"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G102" s="2"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="2"/>
-      <c r="F103" s="2"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G103" s="2"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="2"/>
-      <c r="F104" s="2"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G104" s="2"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="2"/>
-      <c r="F105" s="2"/>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G105" s="2"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="2"/>
-      <c r="F106" s="2"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G106" s="2"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="2"/>
-      <c r="F107" s="2"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G107" s="2"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="2"/>
-      <c r="F108" s="2"/>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G108" s="2"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="2"/>
-      <c r="F109" s="2"/>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G109" s="2"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="2"/>
-      <c r="F110" s="2"/>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G110" s="2"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="2"/>
-      <c r="F111" s="2"/>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G111" s="2"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="2"/>
-      <c r="F112" s="2"/>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G112" s="2"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="2"/>
-      <c r="F113" s="2"/>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G113" s="2"/>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="2"/>
-      <c r="F114" s="2"/>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G114" s="2"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="2"/>
-      <c r="F115" s="2"/>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G115" s="2"/>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="2"/>
-      <c r="F116" s="2"/>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G116" s="2"/>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="2"/>
-      <c r="F117" s="2"/>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G117" s="2"/>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="2"/>
-      <c r="F118" s="2"/>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G118" s="2"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="2"/>
-      <c r="F119" s="2"/>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G119" s="2"/>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="2"/>
-      <c r="F120" s="2"/>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G120" s="2"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="2"/>
-      <c r="F121" s="2"/>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G121" s="2"/>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="2"/>
-      <c r="F122" s="2"/>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G122" s="2"/>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="2"/>
-      <c r="F123" s="2"/>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G123" s="2"/>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="2"/>
-      <c r="F124" s="2"/>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G124" s="2"/>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="2"/>
-      <c r="F125" s="2"/>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G125" s="2"/>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="2"/>
-      <c r="F126" s="2"/>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G126" s="2"/>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="2"/>
-      <c r="F127" s="2"/>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G127" s="2"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="2"/>
-      <c r="F128" s="2"/>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G128" s="2"/>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="2"/>
-      <c r="F129" s="2"/>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G129" s="2"/>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="2"/>
-      <c r="F130" s="2"/>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G130" s="2"/>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="2"/>
-      <c r="F131" s="2"/>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G131" s="2"/>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="2"/>
-      <c r="F132" s="2"/>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G132" s="2"/>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="2"/>
-      <c r="F133" s="2"/>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G133" s="2"/>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="2"/>
-      <c r="F134" s="2"/>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G134" s="2"/>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="2"/>
-      <c r="F135" s="2"/>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G135" s="2"/>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="2"/>
-      <c r="F136" s="2"/>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G136" s="2"/>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="2"/>
-      <c r="F137" s="2"/>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G137" s="2"/>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="2"/>
-      <c r="F138" s="2"/>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G138" s="2"/>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="2"/>
-      <c r="F139" s="2"/>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G139" s="2"/>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="2"/>
-      <c r="F140" s="2"/>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G140" s="2"/>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="2"/>
-      <c r="F141" s="2"/>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G141" s="2"/>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="2"/>
-      <c r="F142" s="2"/>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G142" s="2"/>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="2"/>
-      <c r="F143" s="2"/>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G143" s="2"/>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="2"/>
-      <c r="F144" s="2"/>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G144" s="2"/>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="2"/>
-      <c r="F145" s="2"/>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G145" s="2"/>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="2"/>
-      <c r="F146" s="2"/>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G146" s="2"/>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="2"/>
-      <c r="F147" s="2"/>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G147" s="2"/>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="2"/>
-      <c r="F148" s="2"/>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G148" s="2"/>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="2"/>
-      <c r="F149" s="2"/>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G149" s="2"/>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="2"/>
-      <c r="F150" s="2"/>
+      <c r="G150" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="C1:D1048576">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Notice"</formula>
     </cfRule>
@@ -2061,20 +2234,19 @@
       <formula>"Reject"</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup orientation="landscape" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125978" footer="0.31496062992125978"/>
+  <pageSetup orientation="landscape" horizontalDpi="90" verticalDpi="90"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;G</oddHeader>
   </headerFooter>
-  <legacyDrawingHF r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D5F95FA-2C2D-4B1E-A970-B08C9BD5074E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G200"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2092,29 +2264,45 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -2720,9 +2908,9 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed PMDA from schema, updated reporting services
</commit_message>
<xml_diff>
--- a/resources/templates/report-template.xlsx
+++ b/resources/templates/report-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SamJohnson\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ndedonder\OneDrive - Orange Business (ex-B&amp;D)\CDISC\CORE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{861A05AC-7E66-4324-829A-83AC6D292316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE839BB3-000E-449E-AFCE-7C0B57E39309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14805" yWindow="1050" windowWidth="29400" windowHeight="19305" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conformance Details" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,18 @@
     <sheet name="Issue Details" sheetId="4" r:id="rId4"/>
     <sheet name="Rules Report" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Dataset Details'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Issue Details'!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Issue Summary'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Rules Report'!$A$1:$F$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>Conformance Details</t>
   </si>
@@ -98,12 +104,6 @@
     <t>Explanation</t>
   </si>
   <si>
-    <t>CORE-000334</t>
-  </si>
-  <si>
-    <t>At least one expected variable is missing from dataset</t>
-  </si>
-  <si>
     <t>Executability</t>
   </si>
   <si>
@@ -128,22 +128,13 @@
     <t>FDA RuleID</t>
   </si>
   <si>
-    <t>PMDA RuleID</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>CG0016</t>
-  </si>
-  <si>
-    <t>SUCCESS</t>
-  </si>
-  <si>
     <t>Dataset Domain</t>
+  </si>
+  <si>
+    <t>not configured</t>
   </si>
 </sst>
 </file>
@@ -195,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -209,18 +200,81 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDAA00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDAA00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDAA00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -280,58 +334,6 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFCCE6E3"/>
@@ -348,8 +350,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="CDISC" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="CDISC" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="18"/>
-      <tableStyleElement type="secondRowStripe" dxfId="17"/>
+      <tableStyleElement type="headerRow" dxfId="14"/>
+      <tableStyleElement type="secondRowStripe" dxfId="13"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -361,80 +363,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table4" displayName="Table4" ref="A1:F31" totalsRowShown="0">
-  <autoFilter ref="A1:F31" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Dataset"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Label"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Location"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Modified Time Stamp"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Size (kb)"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Number of Records"/>
-  </tableColumns>
-  <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="A1:F60" totalsRowShown="0">
-  <autoFilter ref="A1:F60" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:F2">
-    <sortCondition ref="B2"/>
-    <sortCondition ref="C2"/>
-  </sortState>
-  <tableColumns count="6">
-    <tableColumn id="4" xr3:uid="{4CBF66AF-B6BA-435A-B965-53A8B1955465}" name="Dataset"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Dataset Domain"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="CORE-ID" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Message" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Issues"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Explanation"/>
-  </tableColumns>
-  <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table1" displayName="Table1" ref="A1:J150" totalsRowShown="0">
-  <autoFilter ref="A1:J150" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J150">
-    <sortCondition ref="A2:A150"/>
-    <sortCondition ref="E2:E150"/>
-    <sortCondition ref="F2:F150"/>
-  </sortState>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="CORE-ID" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Message" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Executability"/>
-    <tableColumn id="10" xr3:uid="{9C910915-7F0C-466C-85EF-3D81E52EA236}" name="Dataset"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Dataset Domain"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="USUBJID"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Record" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Sequence"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Variable(s)" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Value(s)" dataDxfId="10"/>
-  </tableColumns>
-  <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table2" displayName="Table2" ref="A1:G200" totalsRowShown="0">
-  <autoFilter ref="A1:G200" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="CORE-ID" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Version"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="CDISC RuleID"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="FDA RuleID"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="PMDA RuleID"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Message" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Status" dataDxfId="7"/>
-  </tableColumns>
-  <tableStyleInfo name="CDISC" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -734,10 +662,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,10 +676,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="8"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -770,10 +699,10 @@
       <c r="B4"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9"/>
+      <c r="B6" s="8"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -801,25 +730,40 @@
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="B11" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="B12" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="B13" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="B14" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>13</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -828,7 +772,7 @@
     <mergeCell ref="A6:B6"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"not configured"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -839,11 +783,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F29"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -856,22 +799,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1059,61 +1002,19 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F60"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1126,40 +1027,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
@@ -1373,178 +1266,146 @@
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-    </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-    </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-    </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125978" footer="0.31496062992125978"/>
   <pageSetup orientation="landscape" horizontalDpi="90" verticalDpi="90"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;G</oddHeader>
   </headerFooter>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:K150"/>
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:J147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="35.42578125" style="1" customWidth="1"/>
     <col min="10" max="10" width="64.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="1"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="G4" s="2"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="G5" s="2"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="G6" s="2"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="G7" s="2"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="G16" s="2"/>
@@ -2204,33 +2065,19 @@
       <c r="B147" s="2"/>
       <c r="G147" s="2"/>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A148" s="1"/>
-      <c r="B148" s="2"/>
-      <c r="G148" s="2"/>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A149" s="1"/>
-      <c r="B149" s="2"/>
-      <c r="G149" s="2"/>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A150" s="1"/>
-      <c r="B150" s="2"/>
-      <c r="G150" s="2"/>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:J1" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"Notice"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>"Warning"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
       <formula>"Reject"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2239,111 +2086,89 @@
   <headerFooter>
     <oddHeader>&amp;L&amp;G</oddHeader>
   </headerFooter>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G200"/>
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:F197"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="100" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="100" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -2889,28 +2714,17 @@
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" s="1"/>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="1"/>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" s="1"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"SUCCESS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new template, changed filename origin
</commit_message>
<xml_diff>
--- a/resources/templates/report-template.xlsx
+++ b/resources/templates/report-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SamJohnson\Documents\workspaces\cdisc-rules-engine\resources\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NickDeDonder\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C42A8D5-8D8B-4D20-A658-E90C38E3C89B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F280011-466F-4574-9864-135F1268EE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17190" yWindow="5610" windowWidth="32025" windowHeight="15285" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conformance Details" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,10 @@
     <sheet name="Rules Report" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">'Dataset Details'!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3">'Issue Details'!$A$1:$I$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2">'Issue Summary'!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4">'Rules Report'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Dataset Details'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Issue Details'!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Issue Summary'!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Rules Report'!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -270,20 +270,34 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -306,6 +320,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFC94543"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -607,8 +626,8 @@
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,10 +637,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -660,10 +679,10 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="12"/>
+      <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -740,6 +759,11 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A8:B8"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Not configured"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -753,12 +777,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD1048576"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="36" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" style="4" bestFit="1" customWidth="1"/>
@@ -971,6 +995,7 @@
       <c r="F24" s="5"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -984,13 +1009,13 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="4" customWidth="1"/>
     <col min="3" max="3" width="66" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="65.140625" bestFit="1" customWidth="1"/>
@@ -1235,6 +1260,7 @@
       <c r="C56" s="5"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E1" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1249,15 +1275,15 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" activeCellId="1" sqref="A3 A2:XFD1048576"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="1" sqref="A3 A2:XFD1048576"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="59.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
@@ -2031,6 +2057,7 @@
       <c r="F147" s="6"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I1" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2042,19 +2069,19 @@
   </sheetPr>
   <dimension ref="A1:G197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" activeCellId="1" sqref="A3 A2:XFD1048576"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="100" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="103.42578125" style="4" customWidth="1"/>
     <col min="6" max="6" width="21.140625" style="4" customWidth="1"/>
     <col min="7" max="7" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -2075,7 +2102,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="3"/>
@@ -2669,11 +2696,12 @@
       <c r="A197" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:F15 F17 F19:F1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"SUCCESS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
new template, changed filename origin (#1461)
* new template, changed filename origin

* test

* fix report and update env

---------

Co-authored-by: RamilCDISC <113539111+RamilCDISC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/resources/templates/report-template.xlsx
+++ b/resources/templates/report-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SamJohnson\Documents\workspaces\cdisc-rules-engine\resources\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NickDeDonder\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C42A8D5-8D8B-4D20-A658-E90C38E3C89B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F280011-466F-4574-9864-135F1268EE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17190" yWindow="5610" windowWidth="32025" windowHeight="15285" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conformance Details" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,10 @@
     <sheet name="Rules Report" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">'Dataset Details'!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3">'Issue Details'!$A$1:$I$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2">'Issue Summary'!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4">'Rules Report'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Dataset Details'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Issue Details'!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Issue Summary'!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Rules Report'!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -270,20 +270,34 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -306,6 +320,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFC94543"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -607,8 +626,8 @@
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,10 +637,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -660,10 +679,10 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="12"/>
+      <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -740,6 +759,11 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A8:B8"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Not configured"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -753,12 +777,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD1048576"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="36" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" style="4" bestFit="1" customWidth="1"/>
@@ -971,6 +995,7 @@
       <c r="F24" s="5"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -984,13 +1009,13 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="4" customWidth="1"/>
     <col min="3" max="3" width="66" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="65.140625" bestFit="1" customWidth="1"/>
@@ -1235,6 +1260,7 @@
       <c r="C56" s="5"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E1" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1249,15 +1275,15 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" activeCellId="1" sqref="A3 A2:XFD1048576"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="1" sqref="A3 A2:XFD1048576"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="59.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
@@ -2031,6 +2057,7 @@
       <c r="F147" s="6"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I1" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2042,19 +2069,19 @@
   </sheetPr>
   <dimension ref="A1:G197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" activeCellId="1" sqref="A3 A2:XFD1048576"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="100" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="103.42578125" style="4" customWidth="1"/>
     <col min="6" max="6" width="21.140625" style="4" customWidth="1"/>
     <col min="7" max="7" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -2075,7 +2102,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="3"/>
@@ -2669,11 +2696,12 @@
       <c r="A197" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:F15 F17 F19:F1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"SUCCESS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add finer details to execution status
</commit_message>
<xml_diff>
--- a/resources/templates/report-template.xlsx
+++ b/resources/templates/report-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NickDeDonder\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GerryCampion\Code\cdisc-rules-engine\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F280011-466F-4574-9864-135F1268EE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6A743A-FC9A-4A7E-865F-7B3A6C18B2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conformance Details" sheetId="1" r:id="rId1"/>
@@ -283,15 +283,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="9">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC94543"/>
@@ -314,7 +310,64 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDAA00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
         </patternFill>
       </fill>
     </dxf>
@@ -630,34 +683,34 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.44140625" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="13"/>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -665,7 +718,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
@@ -673,23 +726,23 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="13"/>
     </row>
-    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
@@ -697,24 +750,24 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="8"/>
     </row>
-    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B13" s="8"/>
     </row>
-    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
@@ -722,7 +775,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
@@ -730,7 +783,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
@@ -738,7 +791,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>38</v>
       </c>
@@ -746,7 +799,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>39</v>
       </c>
@@ -760,7 +813,7 @@
     <mergeCell ref="A8:B8"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"Not configured"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -780,17 +833,17 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="36" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -810,7 +863,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -818,7 +871,7 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -826,7 +879,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -834,7 +887,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -842,7 +895,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -850,7 +903,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -858,7 +911,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -866,7 +919,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -874,7 +927,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -882,7 +935,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -890,7 +943,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -898,7 +951,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -906,7 +959,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -914,7 +967,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -922,7 +975,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -930,7 +983,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -938,7 +991,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -946,7 +999,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -954,7 +1007,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -962,7 +1015,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -970,7 +1023,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -978,7 +1031,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -986,7 +1039,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1012,16 +1065,16 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="66" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="65.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="65.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1038,224 +1091,224 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
     </row>
-    <row r="38" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
     </row>
-    <row r="39" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
     </row>
-    <row r="40" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
     </row>
-    <row r="41" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
     </row>
-    <row r="42" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
     </row>
-    <row r="43" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
     </row>
-    <row r="44" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
     </row>
-    <row r="45" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
     </row>
-    <row r="46" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
     </row>
-    <row r="47" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
     </row>
-    <row r="48" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
     </row>
-    <row r="49" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
     </row>
-    <row r="50" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
     </row>
-    <row r="51" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
     </row>
-    <row r="52" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
     </row>
-    <row r="53" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
     </row>
-    <row r="54" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
     </row>
-    <row r="55" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
     </row>
-    <row r="56" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
     </row>
@@ -1278,20 +1331,20 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="59.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="59.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="64.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="64.44140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1320,738 +1373,738 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="F2" s="6"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="6"/>
       <c r="F3" s="6"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="F4" s="6"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
       <c r="F5" s="6"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="F6" s="6"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="F7" s="6"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="6"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="6"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="6"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="6"/>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="6"/>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="6"/>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="6"/>
       <c r="F37" s="6"/>
     </row>
-    <row r="38" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="6"/>
       <c r="F38" s="6"/>
     </row>
-    <row r="39" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="6"/>
       <c r="F39" s="6"/>
     </row>
-    <row r="40" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="6"/>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
       <c r="B41" s="6"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
       <c r="B42" s="6"/>
       <c r="F42" s="6"/>
     </row>
-    <row r="43" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
       <c r="B43" s="6"/>
       <c r="F43" s="6"/>
     </row>
-    <row r="44" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
       <c r="B44" s="6"/>
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
       <c r="B45" s="6"/>
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
       <c r="B46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
       <c r="B47" s="6"/>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
       <c r="B48" s="6"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
       <c r="B49" s="6"/>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5"/>
       <c r="B50" s="6"/>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5"/>
       <c r="B51" s="6"/>
       <c r="F51" s="6"/>
     </row>
-    <row r="52" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
       <c r="B52" s="6"/>
       <c r="F52" s="6"/>
     </row>
-    <row r="53" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5"/>
       <c r="B53" s="6"/>
       <c r="F53" s="6"/>
     </row>
-    <row r="54" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5"/>
       <c r="B54" s="6"/>
       <c r="F54" s="6"/>
     </row>
-    <row r="55" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5"/>
       <c r="B55" s="6"/>
       <c r="F55" s="6"/>
     </row>
-    <row r="56" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5"/>
       <c r="B56" s="6"/>
       <c r="F56" s="6"/>
     </row>
-    <row r="57" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5"/>
       <c r="B57" s="6"/>
       <c r="F57" s="6"/>
     </row>
-    <row r="58" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5"/>
       <c r="B58" s="6"/>
       <c r="F58" s="6"/>
     </row>
-    <row r="59" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="5"/>
       <c r="B59" s="6"/>
       <c r="F59" s="6"/>
     </row>
-    <row r="60" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5"/>
       <c r="B60" s="6"/>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="5"/>
       <c r="B61" s="6"/>
       <c r="F61" s="6"/>
     </row>
-    <row r="62" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="5"/>
       <c r="B62" s="6"/>
       <c r="F62" s="6"/>
     </row>
-    <row r="63" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="5"/>
       <c r="B63" s="6"/>
       <c r="F63" s="6"/>
     </row>
-    <row r="64" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="5"/>
       <c r="B64" s="6"/>
       <c r="F64" s="6"/>
     </row>
-    <row r="65" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="5"/>
       <c r="B65" s="6"/>
       <c r="F65" s="6"/>
     </row>
-    <row r="66" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="5"/>
       <c r="B66" s="6"/>
       <c r="F66" s="6"/>
     </row>
-    <row r="67" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="5"/>
       <c r="B67" s="6"/>
       <c r="F67" s="6"/>
     </row>
-    <row r="68" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="5"/>
       <c r="B68" s="6"/>
       <c r="F68" s="6"/>
     </row>
-    <row r="69" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="5"/>
       <c r="B69" s="6"/>
       <c r="F69" s="6"/>
     </row>
-    <row r="70" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="5"/>
       <c r="B70" s="6"/>
       <c r="F70" s="6"/>
     </row>
-    <row r="71" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="5"/>
       <c r="B71" s="6"/>
       <c r="F71" s="6"/>
     </row>
-    <row r="72" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="5"/>
       <c r="B72" s="6"/>
       <c r="F72" s="6"/>
     </row>
-    <row r="73" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="5"/>
       <c r="B73" s="6"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="5"/>
       <c r="B74" s="6"/>
       <c r="F74" s="6"/>
     </row>
-    <row r="75" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="5"/>
       <c r="B75" s="6"/>
       <c r="F75" s="6"/>
     </row>
-    <row r="76" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="5"/>
       <c r="B76" s="6"/>
       <c r="F76" s="6"/>
     </row>
-    <row r="77" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="5"/>
       <c r="B77" s="6"/>
       <c r="F77" s="6"/>
     </row>
-    <row r="78" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="5"/>
       <c r="B78" s="6"/>
       <c r="F78" s="6"/>
     </row>
-    <row r="79" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="5"/>
       <c r="B79" s="6"/>
       <c r="F79" s="6"/>
     </row>
-    <row r="80" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="5"/>
       <c r="B80" s="6"/>
       <c r="F80" s="6"/>
     </row>
-    <row r="81" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="5"/>
       <c r="B81" s="6"/>
       <c r="F81" s="6"/>
     </row>
-    <row r="82" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="5"/>
       <c r="B82" s="6"/>
       <c r="F82" s="6"/>
     </row>
-    <row r="83" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="5"/>
       <c r="B83" s="6"/>
       <c r="F83" s="6"/>
     </row>
-    <row r="84" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="5"/>
       <c r="B84" s="6"/>
       <c r="F84" s="6"/>
     </row>
-    <row r="85" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="5"/>
       <c r="B85" s="6"/>
       <c r="F85" s="6"/>
     </row>
-    <row r="86" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="5"/>
       <c r="B86" s="6"/>
       <c r="F86" s="6"/>
     </row>
-    <row r="87" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="5"/>
       <c r="B87" s="6"/>
       <c r="F87" s="6"/>
     </row>
-    <row r="88" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="5"/>
       <c r="B88" s="6"/>
       <c r="F88" s="6"/>
     </row>
-    <row r="89" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="5"/>
       <c r="B89" s="6"/>
       <c r="F89" s="6"/>
     </row>
-    <row r="90" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="5"/>
       <c r="B90" s="6"/>
       <c r="F90" s="6"/>
     </row>
-    <row r="91" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="5"/>
       <c r="B91" s="6"/>
       <c r="F91" s="6"/>
     </row>
-    <row r="92" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="5"/>
       <c r="B92" s="6"/>
       <c r="F92" s="6"/>
     </row>
-    <row r="93" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="5"/>
       <c r="B93" s="6"/>
       <c r="F93" s="6"/>
     </row>
-    <row r="94" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="5"/>
       <c r="B94" s="6"/>
       <c r="F94" s="6"/>
     </row>
-    <row r="95" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="5"/>
       <c r="B95" s="6"/>
       <c r="F95" s="6"/>
     </row>
-    <row r="96" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="5"/>
       <c r="B96" s="6"/>
       <c r="F96" s="6"/>
     </row>
-    <row r="97" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="5"/>
       <c r="B97" s="6"/>
       <c r="F97" s="6"/>
     </row>
-    <row r="98" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="5"/>
       <c r="B98" s="6"/>
       <c r="F98" s="6"/>
     </row>
-    <row r="99" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="5"/>
       <c r="B99" s="6"/>
       <c r="F99" s="6"/>
     </row>
-    <row r="100" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="5"/>
       <c r="B100" s="6"/>
       <c r="F100" s="6"/>
     </row>
-    <row r="101" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="5"/>
       <c r="B101" s="6"/>
       <c r="F101" s="6"/>
     </row>
-    <row r="102" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="5"/>
       <c r="B102" s="6"/>
       <c r="F102" s="6"/>
     </row>
-    <row r="103" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="5"/>
       <c r="B103" s="6"/>
       <c r="F103" s="6"/>
     </row>
-    <row r="104" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="5"/>
       <c r="B104" s="6"/>
       <c r="F104" s="6"/>
     </row>
-    <row r="105" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="5"/>
       <c r="B105" s="6"/>
       <c r="F105" s="6"/>
     </row>
-    <row r="106" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="5"/>
       <c r="B106" s="6"/>
       <c r="F106" s="6"/>
     </row>
-    <row r="107" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="5"/>
       <c r="B107" s="6"/>
       <c r="F107" s="6"/>
     </row>
-    <row r="108" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="5"/>
       <c r="B108" s="6"/>
       <c r="F108" s="6"/>
     </row>
-    <row r="109" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="5"/>
       <c r="B109" s="6"/>
       <c r="F109" s="6"/>
     </row>
-    <row r="110" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="5"/>
       <c r="B110" s="6"/>
       <c r="F110" s="6"/>
     </row>
-    <row r="111" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="5"/>
       <c r="B111" s="6"/>
       <c r="F111" s="6"/>
     </row>
-    <row r="112" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="5"/>
       <c r="B112" s="6"/>
       <c r="F112" s="6"/>
     </row>
-    <row r="113" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="5"/>
       <c r="B113" s="6"/>
       <c r="F113" s="6"/>
     </row>
-    <row r="114" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="5"/>
       <c r="B114" s="6"/>
       <c r="F114" s="6"/>
     </row>
-    <row r="115" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="5"/>
       <c r="B115" s="6"/>
       <c r="F115" s="6"/>
     </row>
-    <row r="116" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="5"/>
       <c r="B116" s="6"/>
       <c r="F116" s="6"/>
     </row>
-    <row r="117" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="5"/>
       <c r="B117" s="6"/>
       <c r="F117" s="6"/>
     </row>
-    <row r="118" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="5"/>
       <c r="B118" s="6"/>
       <c r="F118" s="6"/>
     </row>
-    <row r="119" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="5"/>
       <c r="B119" s="6"/>
       <c r="F119" s="6"/>
     </row>
-    <row r="120" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="5"/>
       <c r="B120" s="6"/>
       <c r="F120" s="6"/>
     </row>
-    <row r="121" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="5"/>
       <c r="B121" s="6"/>
       <c r="F121" s="6"/>
     </row>
-    <row r="122" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="5"/>
       <c r="B122" s="6"/>
       <c r="F122" s="6"/>
     </row>
-    <row r="123" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="5"/>
       <c r="B123" s="6"/>
       <c r="F123" s="6"/>
     </row>
-    <row r="124" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="5"/>
       <c r="B124" s="6"/>
       <c r="F124" s="6"/>
     </row>
-    <row r="125" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="5"/>
       <c r="B125" s="6"/>
       <c r="F125" s="6"/>
     </row>
-    <row r="126" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="5"/>
       <c r="B126" s="6"/>
       <c r="F126" s="6"/>
     </row>
-    <row r="127" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="5"/>
       <c r="B127" s="6"/>
       <c r="F127" s="6"/>
     </row>
-    <row r="128" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="5"/>
       <c r="B128" s="6"/>
       <c r="F128" s="6"/>
     </row>
-    <row r="129" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="5"/>
       <c r="B129" s="6"/>
       <c r="F129" s="6"/>
     </row>
-    <row r="130" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="5"/>
       <c r="B130" s="6"/>
       <c r="F130" s="6"/>
     </row>
-    <row r="131" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A131" s="5"/>
       <c r="B131" s="6"/>
       <c r="F131" s="6"/>
     </row>
-    <row r="132" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="5"/>
       <c r="B132" s="6"/>
       <c r="F132" s="6"/>
     </row>
-    <row r="133" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="5"/>
       <c r="B133" s="6"/>
       <c r="F133" s="6"/>
     </row>
-    <row r="134" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="5"/>
       <c r="B134" s="6"/>
       <c r="F134" s="6"/>
     </row>
-    <row r="135" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A135" s="5"/>
       <c r="B135" s="6"/>
       <c r="F135" s="6"/>
     </row>
-    <row r="136" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A136" s="5"/>
       <c r="B136" s="6"/>
       <c r="F136" s="6"/>
     </row>
-    <row r="137" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A137" s="5"/>
       <c r="B137" s="6"/>
       <c r="F137" s="6"/>
     </row>
-    <row r="138" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138" s="5"/>
       <c r="B138" s="6"/>
       <c r="F138" s="6"/>
     </row>
-    <row r="139" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A139" s="5"/>
       <c r="B139" s="6"/>
       <c r="F139" s="6"/>
     </row>
-    <row r="140" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140" s="5"/>
       <c r="B140" s="6"/>
       <c r="F140" s="6"/>
     </row>
-    <row r="141" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A141" s="5"/>
       <c r="B141" s="6"/>
       <c r="F141" s="6"/>
     </row>
-    <row r="142" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="5"/>
       <c r="B142" s="6"/>
       <c r="F142" s="6"/>
     </row>
-    <row r="143" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="5"/>
       <c r="B143" s="6"/>
       <c r="F143" s="6"/>
     </row>
-    <row r="144" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="5"/>
       <c r="B144" s="6"/>
       <c r="F144" s="6"/>
     </row>
-    <row r="145" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="5"/>
       <c r="B145" s="6"/>
       <c r="F145" s="6"/>
     </row>
-    <row r="146" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A146" s="5"/>
       <c r="B146" s="6"/>
       <c r="F146" s="6"/>
     </row>
-    <row r="147" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A147" s="5"/>
       <c r="B147" s="6"/>
       <c r="F147" s="6"/>
@@ -2069,24 +2122,24 @@
   </sheetPr>
   <dimension ref="A1:G197"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" activeCellId="1" sqref="A3 A2:XFD1048576"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="103.42578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="103.44140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="26.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2107,604 +2160,611 @@
       </c>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
     </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
     </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
     </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
     </row>
-    <row r="17" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
     </row>
-    <row r="18" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
     </row>
-    <row r="19" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
     </row>
-    <row r="20" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
     </row>
-    <row r="21" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
     </row>
-    <row r="22" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
     </row>
-    <row r="23" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
     </row>
-    <row r="24" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
     </row>
-    <row r="25" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
     </row>
-    <row r="26" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
     </row>
-    <row r="27" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
     </row>
-    <row r="28" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
     </row>
-    <row r="29" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
     </row>
-    <row r="30" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
     </row>
-    <row r="31" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
     </row>
-    <row r="32" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
     </row>
-    <row r="33" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
     </row>
-    <row r="34" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
     </row>
-    <row r="35" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
     </row>
-    <row r="36" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
     </row>
-    <row r="37" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
     </row>
-    <row r="38" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
     </row>
-    <row r="39" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
     </row>
-    <row r="40" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
     </row>
-    <row r="41" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
     </row>
-    <row r="42" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
     </row>
-    <row r="43" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
     </row>
-    <row r="44" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
     </row>
-    <row r="45" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
     </row>
-    <row r="46" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
     </row>
-    <row r="47" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
     </row>
-    <row r="48" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
     </row>
-    <row r="49" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
     </row>
-    <row r="50" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5"/>
     </row>
-    <row r="51" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5"/>
     </row>
-    <row r="52" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
     </row>
-    <row r="53" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5"/>
     </row>
-    <row r="54" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5"/>
     </row>
-    <row r="55" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5"/>
     </row>
-    <row r="56" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5"/>
     </row>
-    <row r="57" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5"/>
     </row>
-    <row r="58" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5"/>
     </row>
-    <row r="59" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="5"/>
     </row>
-    <row r="60" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5"/>
     </row>
-    <row r="61" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="5"/>
     </row>
-    <row r="62" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="5"/>
     </row>
-    <row r="63" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="5"/>
     </row>
-    <row r="64" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="5"/>
     </row>
-    <row r="65" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="5"/>
     </row>
-    <row r="66" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="5"/>
     </row>
-    <row r="67" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="5"/>
     </row>
-    <row r="68" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="5"/>
     </row>
-    <row r="69" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="5"/>
     </row>
-    <row r="70" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="5"/>
     </row>
-    <row r="71" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="5"/>
     </row>
-    <row r="72" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="5"/>
     </row>
-    <row r="73" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="5"/>
     </row>
-    <row r="74" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="5"/>
     </row>
-    <row r="75" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="5"/>
     </row>
-    <row r="76" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="5"/>
     </row>
-    <row r="77" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="5"/>
     </row>
-    <row r="78" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="5"/>
     </row>
-    <row r="79" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="5"/>
     </row>
-    <row r="80" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="5"/>
     </row>
-    <row r="81" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="5"/>
     </row>
-    <row r="82" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="5"/>
     </row>
-    <row r="83" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="5"/>
     </row>
-    <row r="84" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="5"/>
     </row>
-    <row r="85" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="5"/>
     </row>
-    <row r="86" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="5"/>
     </row>
-    <row r="87" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="5"/>
     </row>
-    <row r="88" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="5"/>
     </row>
-    <row r="89" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="5"/>
     </row>
-    <row r="90" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="5"/>
     </row>
-    <row r="91" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="5"/>
     </row>
-    <row r="92" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="5"/>
     </row>
-    <row r="93" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="5"/>
     </row>
-    <row r="94" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="5"/>
     </row>
-    <row r="95" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="5"/>
     </row>
-    <row r="96" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="5"/>
     </row>
-    <row r="97" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="5"/>
     </row>
-    <row r="98" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="5"/>
     </row>
-    <row r="99" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="5"/>
     </row>
-    <row r="100" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="5"/>
     </row>
-    <row r="101" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="5"/>
     </row>
-    <row r="102" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="5"/>
     </row>
-    <row r="103" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="5"/>
     </row>
-    <row r="104" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="5"/>
     </row>
-    <row r="105" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="5"/>
     </row>
-    <row r="106" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="5"/>
     </row>
-    <row r="107" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="5"/>
     </row>
-    <row r="108" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="5"/>
     </row>
-    <row r="109" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="5"/>
     </row>
-    <row r="110" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="5"/>
     </row>
-    <row r="111" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="5"/>
     </row>
-    <row r="112" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="5"/>
     </row>
-    <row r="113" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="5"/>
     </row>
-    <row r="114" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="5"/>
     </row>
-    <row r="115" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="5"/>
     </row>
-    <row r="116" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="5"/>
     </row>
-    <row r="117" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="5"/>
     </row>
-    <row r="118" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="5"/>
     </row>
-    <row r="119" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="5"/>
     </row>
-    <row r="120" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="5"/>
     </row>
-    <row r="121" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="5"/>
     </row>
-    <row r="122" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="5"/>
     </row>
-    <row r="123" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="5"/>
     </row>
-    <row r="124" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="5"/>
     </row>
-    <row r="125" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="5"/>
     </row>
-    <row r="126" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="5"/>
     </row>
-    <row r="127" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="5"/>
     </row>
-    <row r="128" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="5"/>
     </row>
-    <row r="129" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="5"/>
     </row>
-    <row r="130" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="5"/>
     </row>
-    <row r="131" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A131" s="5"/>
     </row>
-    <row r="132" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="5"/>
     </row>
-    <row r="133" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="5"/>
     </row>
-    <row r="134" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="5"/>
     </row>
-    <row r="135" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A135" s="5"/>
     </row>
-    <row r="136" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A136" s="5"/>
     </row>
-    <row r="137" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A137" s="5"/>
     </row>
-    <row r="138" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138" s="5"/>
     </row>
-    <row r="139" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A139" s="5"/>
     </row>
-    <row r="140" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140" s="5"/>
     </row>
-    <row r="141" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A141" s="5"/>
     </row>
-    <row r="142" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="5"/>
     </row>
-    <row r="143" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="5"/>
     </row>
-    <row r="144" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="5"/>
     </row>
-    <row r="145" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="5"/>
     </row>
-    <row r="146" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A146" s="5"/>
     </row>
-    <row r="147" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A147" s="5"/>
     </row>
-    <row r="148" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A148" s="5"/>
     </row>
-    <row r="149" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A149" s="5"/>
     </row>
-    <row r="150" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A150" s="5"/>
     </row>
-    <row r="151" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A151" s="5"/>
     </row>
-    <row r="152" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A152" s="5"/>
     </row>
-    <row r="153" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A153" s="5"/>
     </row>
-    <row r="154" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A154" s="5"/>
     </row>
-    <row r="155" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A155" s="5"/>
     </row>
-    <row r="156" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A156" s="5"/>
     </row>
-    <row r="157" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A157" s="5"/>
     </row>
-    <row r="158" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A158" s="5"/>
     </row>
-    <row r="159" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A159" s="5"/>
     </row>
-    <row r="160" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A160" s="5"/>
     </row>
-    <row r="161" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A161" s="5"/>
     </row>
-    <row r="162" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A162" s="5"/>
     </row>
-    <row r="163" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A163" s="5"/>
     </row>
-    <row r="164" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A164" s="5"/>
     </row>
-    <row r="165" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A165" s="5"/>
     </row>
-    <row r="166" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A166" s="5"/>
     </row>
-    <row r="167" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A167" s="5"/>
     </row>
-    <row r="168" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A168" s="5"/>
     </row>
-    <row r="169" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A169" s="5"/>
     </row>
-    <row r="170" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A170" s="5"/>
     </row>
-    <row r="171" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A171" s="5"/>
     </row>
-    <row r="172" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A172" s="5"/>
     </row>
-    <row r="173" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A173" s="5"/>
     </row>
-    <row r="174" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A174" s="5"/>
     </row>
-    <row r="175" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A175" s="5"/>
     </row>
-    <row r="176" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A176" s="5"/>
     </row>
-    <row r="177" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A177" s="5"/>
     </row>
-    <row r="178" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A178" s="5"/>
     </row>
-    <row r="179" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A179" s="5"/>
     </row>
-    <row r="180" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A180" s="5"/>
     </row>
-    <row r="181" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A181" s="5"/>
     </row>
-    <row r="182" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A182" s="5"/>
     </row>
-    <row r="183" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A183" s="5"/>
     </row>
-    <row r="184" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A184" s="5"/>
     </row>
-    <row r="185" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A185" s="5"/>
     </row>
-    <row r="186" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A186" s="5"/>
     </row>
-    <row r="187" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A187" s="5"/>
     </row>
-    <row r="188" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A188" s="5"/>
     </row>
-    <row r="189" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A189" s="5"/>
     </row>
-    <row r="190" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A190" s="5"/>
     </row>
-    <row r="191" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A191" s="5"/>
     </row>
-    <row r="192" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A192" s="5"/>
     </row>
-    <row r="193" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A193" s="5"/>
     </row>
-    <row r="194" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A194" s="5"/>
     </row>
-    <row r="195" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A195" s="5"/>
     </row>
-    <row r="196" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A196" s="5"/>
     </row>
-    <row r="197" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A197" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"SUCCESS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"SKIPPED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"ISSUE_REPORTED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>"EXECUTION_ERROR"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TIG use case (#1556)
* initial commit tig use case

* validation arg

* use case test

* last test failure

* readme

* report tests, update

* use case ruletester

* fix parsing issue

* update
</commit_message>
<xml_diff>
--- a/resources/templates/report-template.xlsx
+++ b/resources/templates/report-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NickDeDonder\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SamJohnson\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F280011-466F-4574-9864-135F1268EE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EC088E-B95E-4A5D-B44A-79DAB7471C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37665" yWindow="3465" windowWidth="22395" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conformance Details" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>CORE-ID</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>SNOMED Version</t>
+  </si>
+  <si>
+    <t>TIG Use Case</t>
+  </si>
+  <si>
+    <t>LOINC Version</t>
   </si>
 </sst>
 </file>
@@ -283,21 +289,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color auto="1"/>
@@ -315,6 +307,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
         </patternFill>
       </fill>
     </dxf>
@@ -624,10 +623,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,27 +703,27 @@
     </row>
     <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="8"/>
+        <v>40</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="8"/>
     </row>
     <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>35</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B14" s="8"/>
     </row>
     <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>35</v>
@@ -732,7 +731,7 @@
     </row>
     <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>35</v>
@@ -740,7 +739,7 @@
     </row>
     <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>35</v>
@@ -748,9 +747,25 @@
     </row>
     <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B19" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>35</v>
       </c>
     </row>
@@ -760,7 +775,7 @@
     <mergeCell ref="A8:B8"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Not configured"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2698,10 +2713,10 @@
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"SUCCESS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
merge main report-template changes
</commit_message>
<xml_diff>
--- a/resources/templates/report-template.xlsx
+++ b/resources/templates/report-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GerryCampion\Code\cdisc-rules-engine\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6A743A-FC9A-4A7E-865F-7B3A6C18B2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB8E000-29C2-4B48-85B2-774DCD3DB1C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conformance Details" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>CORE-ID</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>SNOMED Version</t>
+  </si>
+  <si>
+    <t>TIG Use Case</t>
+  </si>
+  <si>
+    <t>LOINC Version</t>
   </si>
 </sst>
 </file>
@@ -283,11 +289,8 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="7">
     <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC94543"/>
@@ -295,32 +298,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFEDAA00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor rgb="FFC94543"/>
         </patternFill>
       </fill>
     </dxf>
@@ -677,40 +657,40 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.42578125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="13"/>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -718,7 +698,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
@@ -726,23 +706,23 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="13"/>
     </row>
-    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
@@ -750,60 +730,76 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="8"/>
-    </row>
-    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="8"/>
+    </row>
+    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="8"/>
-    </row>
-    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="8"/>
+    </row>
+    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B19" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>35</v>
       </c>
     </row>
@@ -812,8 +808,18 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A8:B8"/>
   </mergeCells>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+  <conditionalFormatting sqref="B1:B11 B13:B19 B21:B1048576">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+      <formula>"Not configured"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Not configured"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Not configured"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -833,17 +839,17 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="36" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -863,7 +869,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -871,7 +877,7 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -879,7 +885,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -887,7 +893,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -895,7 +901,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -903,7 +909,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -911,7 +917,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -919,7 +925,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -927,7 +933,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -935,7 +941,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -943,7 +949,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -951,7 +957,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -959,7 +965,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -967,7 +973,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -975,7 +981,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -983,7 +989,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -991,7 +997,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -999,7 +1005,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1007,7 +1013,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1015,7 +1021,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1023,7 +1029,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1031,7 +1037,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1039,7 +1045,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1065,16 +1071,16 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="4" customWidth="1"/>
     <col min="3" max="3" width="66" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="65.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="65.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1091,224 +1097,224 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
     </row>
-    <row r="38" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
     </row>
-    <row r="39" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
     </row>
-    <row r="40" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
     </row>
-    <row r="41" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
     </row>
-    <row r="42" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
     </row>
-    <row r="43" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
     </row>
-    <row r="44" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
     </row>
-    <row r="45" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
     </row>
-    <row r="46" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
     </row>
-    <row r="47" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
     </row>
-    <row r="48" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
     </row>
-    <row r="49" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
     </row>
-    <row r="50" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
     </row>
-    <row r="51" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
     </row>
-    <row r="52" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
     </row>
-    <row r="53" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
     </row>
-    <row r="54" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
     </row>
-    <row r="55" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
     </row>
-    <row r="56" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
     </row>
@@ -1331,20 +1337,20 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="59.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="59.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="64.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="64.42578125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1373,738 +1379,738 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="F2" s="6"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="6"/>
       <c r="F3" s="6"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="F4" s="6"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
       <c r="F5" s="6"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="F6" s="6"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="F7" s="6"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="6"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="6"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="6"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="6"/>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="6"/>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="6"/>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="6"/>
       <c r="F37" s="6"/>
     </row>
-    <row r="38" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="6"/>
       <c r="F38" s="6"/>
     </row>
-    <row r="39" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="6"/>
       <c r="F39" s="6"/>
     </row>
-    <row r="40" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="6"/>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="6"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="6"/>
       <c r="F42" s="6"/>
     </row>
-    <row r="43" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="6"/>
       <c r="F43" s="6"/>
     </row>
-    <row r="44" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="6"/>
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="6"/>
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="6"/>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="6"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="6"/>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="6"/>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="6"/>
       <c r="F51" s="6"/>
     </row>
-    <row r="52" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="6"/>
       <c r="F52" s="6"/>
     </row>
-    <row r="53" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="6"/>
       <c r="F53" s="6"/>
     </row>
-    <row r="54" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="6"/>
       <c r="F54" s="6"/>
     </row>
-    <row r="55" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="6"/>
       <c r="F55" s="6"/>
     </row>
-    <row r="56" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="6"/>
       <c r="F56" s="6"/>
     </row>
-    <row r="57" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="6"/>
       <c r="F57" s="6"/>
     </row>
-    <row r="58" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="6"/>
       <c r="F58" s="6"/>
     </row>
-    <row r="59" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
       <c r="B59" s="6"/>
       <c r="F59" s="6"/>
     </row>
-    <row r="60" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="B60" s="6"/>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="6"/>
       <c r="F61" s="6"/>
     </row>
-    <row r="62" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="6"/>
       <c r="F62" s="6"/>
     </row>
-    <row r="63" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="6"/>
       <c r="F63" s="6"/>
     </row>
-    <row r="64" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="B64" s="6"/>
       <c r="F64" s="6"/>
     </row>
-    <row r="65" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="6"/>
       <c r="F65" s="6"/>
     </row>
-    <row r="66" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="B66" s="6"/>
       <c r="F66" s="6"/>
     </row>
-    <row r="67" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="6"/>
       <c r="F67" s="6"/>
     </row>
-    <row r="68" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="B68" s="6"/>
       <c r="F68" s="6"/>
     </row>
-    <row r="69" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="6"/>
       <c r="F69" s="6"/>
     </row>
-    <row r="70" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="6"/>
       <c r="F70" s="6"/>
     </row>
-    <row r="71" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="6"/>
       <c r="F71" s="6"/>
     </row>
-    <row r="72" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="6"/>
       <c r="F72" s="6"/>
     </row>
-    <row r="73" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="6"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="6"/>
       <c r="F74" s="6"/>
     </row>
-    <row r="75" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="6"/>
       <c r="F75" s="6"/>
     </row>
-    <row r="76" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
       <c r="B76" s="6"/>
       <c r="F76" s="6"/>
     </row>
-    <row r="77" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="B77" s="6"/>
       <c r="F77" s="6"/>
     </row>
-    <row r="78" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="B78" s="6"/>
       <c r="F78" s="6"/>
     </row>
-    <row r="79" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="B79" s="6"/>
       <c r="F79" s="6"/>
     </row>
-    <row r="80" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="B80" s="6"/>
       <c r="F80" s="6"/>
     </row>
-    <row r="81" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="B81" s="6"/>
       <c r="F81" s="6"/>
     </row>
-    <row r="82" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
       <c r="B82" s="6"/>
       <c r="F82" s="6"/>
     </row>
-    <row r="83" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
       <c r="B83" s="6"/>
       <c r="F83" s="6"/>
     </row>
-    <row r="84" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
       <c r="B84" s="6"/>
       <c r="F84" s="6"/>
     </row>
-    <row r="85" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
       <c r="B85" s="6"/>
       <c r="F85" s="6"/>
     </row>
-    <row r="86" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
       <c r="B86" s="6"/>
       <c r="F86" s="6"/>
     </row>
-    <row r="87" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
       <c r="B87" s="6"/>
       <c r="F87" s="6"/>
     </row>
-    <row r="88" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
       <c r="B88" s="6"/>
       <c r="F88" s="6"/>
     </row>
-    <row r="89" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="B89" s="6"/>
       <c r="F89" s="6"/>
     </row>
-    <row r="90" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5"/>
       <c r="B90" s="6"/>
       <c r="F90" s="6"/>
     </row>
-    <row r="91" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
       <c r="B91" s="6"/>
       <c r="F91" s="6"/>
     </row>
-    <row r="92" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5"/>
       <c r="B92" s="6"/>
       <c r="F92" s="6"/>
     </row>
-    <row r="93" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="5"/>
       <c r="B93" s="6"/>
       <c r="F93" s="6"/>
     </row>
-    <row r="94" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="5"/>
       <c r="B94" s="6"/>
       <c r="F94" s="6"/>
     </row>
-    <row r="95" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
       <c r="B95" s="6"/>
       <c r="F95" s="6"/>
     </row>
-    <row r="96" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="5"/>
       <c r="B96" s="6"/>
       <c r="F96" s="6"/>
     </row>
-    <row r="97" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="5"/>
       <c r="B97" s="6"/>
       <c r="F97" s="6"/>
     </row>
-    <row r="98" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="5"/>
       <c r="B98" s="6"/>
       <c r="F98" s="6"/>
     </row>
-    <row r="99" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
       <c r="B99" s="6"/>
       <c r="F99" s="6"/>
     </row>
-    <row r="100" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="5"/>
       <c r="B100" s="6"/>
       <c r="F100" s="6"/>
     </row>
-    <row r="101" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
       <c r="B101" s="6"/>
       <c r="F101" s="6"/>
     </row>
-    <row r="102" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="5"/>
       <c r="B102" s="6"/>
       <c r="F102" s="6"/>
     </row>
-    <row r="103" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="5"/>
       <c r="B103" s="6"/>
       <c r="F103" s="6"/>
     </row>
-    <row r="104" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
       <c r="B104" s="6"/>
       <c r="F104" s="6"/>
     </row>
-    <row r="105" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="5"/>
       <c r="B105" s="6"/>
       <c r="F105" s="6"/>
     </row>
-    <row r="106" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="5"/>
       <c r="B106" s="6"/>
       <c r="F106" s="6"/>
     </row>
-    <row r="107" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="5"/>
       <c r="B107" s="6"/>
       <c r="F107" s="6"/>
     </row>
-    <row r="108" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="5"/>
       <c r="B108" s="6"/>
       <c r="F108" s="6"/>
     </row>
-    <row r="109" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="5"/>
       <c r="B109" s="6"/>
       <c r="F109" s="6"/>
     </row>
-    <row r="110" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="5"/>
       <c r="B110" s="6"/>
       <c r="F110" s="6"/>
     </row>
-    <row r="111" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
       <c r="B111" s="6"/>
       <c r="F111" s="6"/>
     </row>
-    <row r="112" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="5"/>
       <c r="B112" s="6"/>
       <c r="F112" s="6"/>
     </row>
-    <row r="113" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="5"/>
       <c r="B113" s="6"/>
       <c r="F113" s="6"/>
     </row>
-    <row r="114" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="5"/>
       <c r="B114" s="6"/>
       <c r="F114" s="6"/>
     </row>
-    <row r="115" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="5"/>
       <c r="B115" s="6"/>
       <c r="F115" s="6"/>
     </row>
-    <row r="116" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="5"/>
       <c r="B116" s="6"/>
       <c r="F116" s="6"/>
     </row>
-    <row r="117" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="5"/>
       <c r="B117" s="6"/>
       <c r="F117" s="6"/>
     </row>
-    <row r="118" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="5"/>
       <c r="B118" s="6"/>
       <c r="F118" s="6"/>
     </row>
-    <row r="119" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="5"/>
       <c r="B119" s="6"/>
       <c r="F119" s="6"/>
     </row>
-    <row r="120" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="5"/>
       <c r="B120" s="6"/>
       <c r="F120" s="6"/>
     </row>
-    <row r="121" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="5"/>
       <c r="B121" s="6"/>
       <c r="F121" s="6"/>
     </row>
-    <row r="122" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="5"/>
       <c r="B122" s="6"/>
       <c r="F122" s="6"/>
     </row>
-    <row r="123" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="5"/>
       <c r="B123" s="6"/>
       <c r="F123" s="6"/>
     </row>
-    <row r="124" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="5"/>
       <c r="B124" s="6"/>
       <c r="F124" s="6"/>
     </row>
-    <row r="125" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="5"/>
       <c r="B125" s="6"/>
       <c r="F125" s="6"/>
     </row>
-    <row r="126" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="5"/>
       <c r="B126" s="6"/>
       <c r="F126" s="6"/>
     </row>
-    <row r="127" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="5"/>
       <c r="B127" s="6"/>
       <c r="F127" s="6"/>
     </row>
-    <row r="128" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="5"/>
       <c r="B128" s="6"/>
       <c r="F128" s="6"/>
     </row>
-    <row r="129" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="5"/>
       <c r="B129" s="6"/>
       <c r="F129" s="6"/>
     </row>
-    <row r="130" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="5"/>
       <c r="B130" s="6"/>
       <c r="F130" s="6"/>
     </row>
-    <row r="131" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="5"/>
       <c r="B131" s="6"/>
       <c r="F131" s="6"/>
     </row>
-    <row r="132" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="5"/>
       <c r="B132" s="6"/>
       <c r="F132" s="6"/>
     </row>
-    <row r="133" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="5"/>
       <c r="B133" s="6"/>
       <c r="F133" s="6"/>
     </row>
-    <row r="134" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="5"/>
       <c r="B134" s="6"/>
       <c r="F134" s="6"/>
     </row>
-    <row r="135" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="5"/>
       <c r="B135" s="6"/>
       <c r="F135" s="6"/>
     </row>
-    <row r="136" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="5"/>
       <c r="B136" s="6"/>
       <c r="F136" s="6"/>
     </row>
-    <row r="137" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="5"/>
       <c r="B137" s="6"/>
       <c r="F137" s="6"/>
     </row>
-    <row r="138" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="5"/>
       <c r="B138" s="6"/>
       <c r="F138" s="6"/>
     </row>
-    <row r="139" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="5"/>
       <c r="B139" s="6"/>
       <c r="F139" s="6"/>
     </row>
-    <row r="140" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="5"/>
       <c r="B140" s="6"/>
       <c r="F140" s="6"/>
     </row>
-    <row r="141" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="5"/>
       <c r="B141" s="6"/>
       <c r="F141" s="6"/>
     </row>
-    <row r="142" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="5"/>
       <c r="B142" s="6"/>
       <c r="F142" s="6"/>
     </row>
-    <row r="143" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="5"/>
       <c r="B143" s="6"/>
       <c r="F143" s="6"/>
     </row>
-    <row r="144" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="5"/>
       <c r="B144" s="6"/>
       <c r="F144" s="6"/>
     </row>
-    <row r="145" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="5"/>
       <c r="B145" s="6"/>
       <c r="F145" s="6"/>
     </row>
-    <row r="146" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="5"/>
       <c r="B146" s="6"/>
       <c r="F146" s="6"/>
     </row>
-    <row r="147" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="5"/>
       <c r="B147" s="6"/>
       <c r="F147" s="6"/>
@@ -2128,18 +2134,18 @@
       <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
-    <col min="5" max="5" width="103.44140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="103.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2160,607 +2166,607 @@
       </c>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
     </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
     </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
     </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
     </row>
-    <row r="17" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
     </row>
-    <row r="18" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
     </row>
-    <row r="19" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
     </row>
-    <row r="20" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
     </row>
-    <row r="21" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
     </row>
-    <row r="22" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
     </row>
-    <row r="23" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
     </row>
-    <row r="24" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
     </row>
-    <row r="25" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
     </row>
-    <row r="26" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
     </row>
-    <row r="27" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
     </row>
-    <row r="28" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
     </row>
-    <row r="29" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
     </row>
-    <row r="30" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
     </row>
-    <row r="31" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
     </row>
-    <row r="32" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
     </row>
-    <row r="33" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
     </row>
-    <row r="34" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
     </row>
-    <row r="35" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
     </row>
-    <row r="36" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
     </row>
-    <row r="37" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
     </row>
-    <row r="38" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
     </row>
-    <row r="39" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
     </row>
-    <row r="40" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
     </row>
-    <row r="41" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
     </row>
-    <row r="42" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
     </row>
-    <row r="43" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
     </row>
-    <row r="44" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
     </row>
-    <row r="45" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
     </row>
-    <row r="46" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
     </row>
-    <row r="47" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
     </row>
-    <row r="48" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
     </row>
-    <row r="49" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
     </row>
-    <row r="50" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
     </row>
-    <row r="51" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
     </row>
-    <row r="52" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
     </row>
-    <row r="53" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
     </row>
-    <row r="54" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
     </row>
-    <row r="55" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
     </row>
-    <row r="56" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
     </row>
-    <row r="57" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
     </row>
-    <row r="58" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
     </row>
-    <row r="59" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
     </row>
-    <row r="60" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
     </row>
-    <row r="61" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
     </row>
-    <row r="62" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
     </row>
-    <row r="63" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
     </row>
-    <row r="64" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
     </row>
-    <row r="65" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
     </row>
-    <row r="66" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
     </row>
-    <row r="67" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
     </row>
-    <row r="68" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
     </row>
-    <row r="69" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
     </row>
-    <row r="70" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
     </row>
-    <row r="71" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
     </row>
-    <row r="72" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
     </row>
-    <row r="73" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
     </row>
-    <row r="74" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
     </row>
-    <row r="75" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
     </row>
-    <row r="76" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
     </row>
-    <row r="77" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
     </row>
-    <row r="78" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
     </row>
-    <row r="79" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
     </row>
-    <row r="80" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
     </row>
-    <row r="81" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
     </row>
-    <row r="82" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
     </row>
-    <row r="83" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
     </row>
-    <row r="84" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
     </row>
-    <row r="85" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
     </row>
-    <row r="86" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
     </row>
-    <row r="87" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
     </row>
-    <row r="88" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
     </row>
-    <row r="89" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
     </row>
-    <row r="90" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5"/>
     </row>
-    <row r="91" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
     </row>
-    <row r="92" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5"/>
     </row>
-    <row r="93" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="5"/>
     </row>
-    <row r="94" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="5"/>
     </row>
-    <row r="95" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
     </row>
-    <row r="96" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="5"/>
     </row>
-    <row r="97" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="5"/>
     </row>
-    <row r="98" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="5"/>
     </row>
-    <row r="99" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
     </row>
-    <row r="100" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="5"/>
     </row>
-    <row r="101" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
     </row>
-    <row r="102" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="5"/>
     </row>
-    <row r="103" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="5"/>
     </row>
-    <row r="104" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
     </row>
-    <row r="105" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="5"/>
     </row>
-    <row r="106" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="5"/>
     </row>
-    <row r="107" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="5"/>
     </row>
-    <row r="108" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="5"/>
     </row>
-    <row r="109" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="5"/>
     </row>
-    <row r="110" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="5"/>
     </row>
-    <row r="111" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
     </row>
-    <row r="112" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="5"/>
     </row>
-    <row r="113" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="5"/>
     </row>
-    <row r="114" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="5"/>
     </row>
-    <row r="115" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="5"/>
     </row>
-    <row r="116" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="5"/>
     </row>
-    <row r="117" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="5"/>
     </row>
-    <row r="118" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="5"/>
     </row>
-    <row r="119" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="5"/>
     </row>
-    <row r="120" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="5"/>
     </row>
-    <row r="121" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="5"/>
     </row>
-    <row r="122" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="5"/>
     </row>
-    <row r="123" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="5"/>
     </row>
-    <row r="124" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="5"/>
     </row>
-    <row r="125" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="5"/>
     </row>
-    <row r="126" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="5"/>
     </row>
-    <row r="127" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="5"/>
     </row>
-    <row r="128" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="5"/>
     </row>
-    <row r="129" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="5"/>
     </row>
-    <row r="130" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="5"/>
     </row>
-    <row r="131" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="5"/>
     </row>
-    <row r="132" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="5"/>
     </row>
-    <row r="133" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="5"/>
     </row>
-    <row r="134" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="5"/>
     </row>
-    <row r="135" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="5"/>
     </row>
-    <row r="136" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="5"/>
     </row>
-    <row r="137" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="5"/>
     </row>
-    <row r="138" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="5"/>
     </row>
-    <row r="139" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="5"/>
     </row>
-    <row r="140" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="5"/>
     </row>
-    <row r="141" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="5"/>
     </row>
-    <row r="142" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="5"/>
     </row>
-    <row r="143" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="5"/>
     </row>
-    <row r="144" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="5"/>
     </row>
-    <row r="145" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="5"/>
     </row>
-    <row r="146" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="5"/>
     </row>
-    <row r="147" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="5"/>
     </row>
-    <row r="148" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="5"/>
     </row>
-    <row r="149" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="5"/>
     </row>
-    <row r="150" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="5"/>
     </row>
-    <row r="151" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="5"/>
     </row>
-    <row r="152" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="5"/>
     </row>
-    <row r="153" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="5"/>
     </row>
-    <row r="154" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="5"/>
     </row>
-    <row r="155" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="5"/>
     </row>
-    <row r="156" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="5"/>
     </row>
-    <row r="157" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="5"/>
     </row>
-    <row r="158" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="5"/>
     </row>
-    <row r="159" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="5"/>
     </row>
-    <row r="160" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="5"/>
     </row>
-    <row r="161" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="5"/>
     </row>
-    <row r="162" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="5"/>
     </row>
-    <row r="163" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="5"/>
     </row>
-    <row r="164" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="5"/>
     </row>
-    <row r="165" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="5"/>
     </row>
-    <row r="166" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="5"/>
     </row>
-    <row r="167" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="5"/>
     </row>
-    <row r="168" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="5"/>
     </row>
-    <row r="169" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="5"/>
     </row>
-    <row r="170" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="5"/>
     </row>
-    <row r="171" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="5"/>
     </row>
-    <row r="172" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="5"/>
     </row>
-    <row r="173" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A173" s="5"/>
     </row>
-    <row r="174" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="5"/>
     </row>
-    <row r="175" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="5"/>
     </row>
-    <row r="176" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="5"/>
     </row>
-    <row r="177" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="5"/>
     </row>
-    <row r="178" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A178" s="5"/>
     </row>
-    <row r="179" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="5"/>
     </row>
-    <row r="180" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="5"/>
     </row>
-    <row r="181" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A181" s="5"/>
     </row>
-    <row r="182" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A182" s="5"/>
     </row>
-    <row r="183" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A183" s="5"/>
     </row>
-    <row r="184" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="5"/>
     </row>
-    <row r="185" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="5"/>
     </row>
-    <row r="186" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="5"/>
     </row>
-    <row r="187" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A187" s="5"/>
     </row>
-    <row r="188" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A188" s="5"/>
     </row>
-    <row r="189" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A189" s="5"/>
     </row>
-    <row r="190" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A190" s="5"/>
     </row>
-    <row r="191" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="5"/>
     </row>
-    <row r="192" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A192" s="5"/>
     </row>
-    <row r="193" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A193" s="5"/>
     </row>
-    <row r="194" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="5"/>
     </row>
-    <row r="195" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="5"/>
     </row>
-    <row r="196" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="5"/>
     </row>
-    <row r="197" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"SUCCESS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"ISSUE_REPORTED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"EXECUTION_ERROR"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
471 improved issue reporting (#1551)
* Add finer details to execution status

* reorg skips and execution errors

* skip reasons and better execution error categorization

* error dask parquet filename fix

* fix dask meta issue

* make date parser error a rule execution error instead of skip

* dataset_preprocessor.py lint update

* Fix issue summary tab

* merge main report-template changes

---------

Co-authored-by: Samuel Johnson <96841389+SFJohnson24@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/resources/templates/report-template.xlsx
+++ b/resources/templates/report-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SamJohnson\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GerryCampion\Code\cdisc-rules-engine\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EC088E-B95E-4A5D-B44A-79DAB7471C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB8E000-29C2-4B48-85B2-774DCD3DB1C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37665" yWindow="3465" windowWidth="22395" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conformance Details" sheetId="1" r:id="rId1"/>
@@ -289,7 +289,31 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC94543"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -297,6 +321,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFEDAA00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -626,7 +660,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,8 +808,18 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A8:B8"/>
   </mergeCells>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <conditionalFormatting sqref="B1:B11 B13:B19 B21:B1048576">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+      <formula>"Not configured"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Not configured"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Not configured"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2084,10 +2128,10 @@
   </sheetPr>
   <dimension ref="A1:G197"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" activeCellId="1" sqref="A3 A2:XFD1048576"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2713,13 +2757,20 @@
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"SUCCESS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"SKIPPED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"ISSUE_REPORTED"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"EXECUTION_ERROR"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
rule type, builder changes
</commit_message>
<xml_diff>
--- a/resources/templates/report-template.xlsx
+++ b/resources/templates/report-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GerryCampion\Code\cdisc-rules-engine\resources\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SamJohnson\Documents\workspaces\cdisc-rules-engine\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB8E000-29C2-4B48-85B2-774DCD3DB1C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046EE3FE-2108-4134-83E6-35D5975BD6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15930" yWindow="2730" windowWidth="30480" windowHeight="14475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conformance Details" sheetId="1" r:id="rId1"/>
@@ -269,9 +269,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -285,25 +282,12 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC94543"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color auto="1"/>
@@ -660,20 +644,20 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.42578125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -694,7 +678,7 @@
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -702,7 +686,7 @@
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -712,10 +696,10 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="13"/>
+      <c r="B8" s="12"/>
     </row>
     <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -726,7 +710,7 @@
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -739,7 +723,7 @@
       <c r="A12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -747,19 +731,19 @@
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="13"/>
     </row>
     <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="13"/>
     </row>
     <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>35</v>
       </c>
     </row>
@@ -767,7 +751,7 @@
       <c r="A16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>35</v>
       </c>
     </row>
@@ -775,7 +759,7 @@
       <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>35</v>
       </c>
     </row>
@@ -783,7 +767,7 @@
       <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>35</v>
       </c>
     </row>
@@ -791,7 +775,7 @@
       <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>35</v>
       </c>
     </row>
@@ -799,7 +783,7 @@
       <c r="A20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>35</v>
       </c>
     </row>
@@ -808,18 +792,8 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A8:B8"/>
   </mergeCells>
-  <conditionalFormatting sqref="B1:B11 B13:B19 B21:B1048576">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
-      <formula>"Not configured"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B12">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"Not configured"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"Not configured"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2161,7 +2135,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="3"/>
@@ -2757,16 +2731,16 @@
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"SUCCESS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"SKIPPED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"ISSUE_REPORTED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"EXECUTION_ERROR"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>